<commit_message>
Add punctuation counter and update analysis
</commit_message>
<xml_diff>
--- a/New Analysis.xlsx
+++ b/New Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="All Results" sheetId="1" r:id="rId1"/>
@@ -920,13 +920,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9329,13 +9329,13 @@
       <c r="C5" s="3">
         <v>0.15</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9347,9 +9347,9 @@
       <c r="C6" s="3">
         <v>0.15</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -9430,13 +9430,13 @@
       <c r="C15" s="3">
         <v>0.15</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9448,9 +9448,9 @@
       <c r="C16" s="3">
         <v>0.15</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="47"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
@@ -9531,13 +9531,13 @@
       <c r="C25" s="3">
         <v>0.12</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="49" t="s">
+      <c r="F25" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9549,9 +9549,9 @@
       <c r="C26" s="3">
         <v>0.12</v>
       </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="47"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
@@ -9638,7 +9638,7 @@
       <c r="E35" s="10">
         <v>49630</v>
       </c>
-      <c r="F35" s="49" t="s">
+      <c r="F35" s="47" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9656,7 +9656,7 @@
       <c r="E36" s="10">
         <v>49479</v>
       </c>
-      <c r="F36" s="49"/>
+      <c r="F36" s="47"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
@@ -9737,13 +9737,13 @@
       <c r="C45" s="3">
         <v>0.15</v>
       </c>
-      <c r="D45" s="49" t="s">
+      <c r="D45" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="47" t="s">
+      <c r="E45" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="49" t="s">
+      <c r="F45" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9755,9 +9755,9 @@
       <c r="C46" s="3">
         <v>0.15</v>
       </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="49"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="47"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
@@ -9838,13 +9838,13 @@
       <c r="C55" s="3">
         <v>0.15</v>
       </c>
-      <c r="D55" s="49" t="s">
+      <c r="D55" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="47" t="s">
+      <c r="E55" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="49" t="s">
+      <c r="F55" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9856,9 +9856,9 @@
       <c r="C56" s="3">
         <v>0.15</v>
       </c>
-      <c r="D56" s="49"/>
-      <c r="E56" s="48"/>
-      <c r="F56" s="49"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="47"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
@@ -9942,13 +9942,13 @@
       <c r="C65" s="3">
         <v>0.15</v>
       </c>
-      <c r="D65" s="49" t="s">
+      <c r="D65" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="47" t="s">
+      <c r="E65" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="49" t="s">
+      <c r="F65" s="47" t="s">
         <v>32</v>
       </c>
       <c r="G65" s="17"/>
@@ -9961,9 +9961,9 @@
       <c r="C66" s="3">
         <v>0.15</v>
       </c>
-      <c r="D66" s="49"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="49"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="47"/>
       <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -10055,13 +10055,13 @@
       <c r="C75" s="3">
         <v>0.15</v>
       </c>
-      <c r="D75" s="49" t="s">
+      <c r="D75" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="47" t="s">
+      <c r="E75" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F75" s="49" t="s">
+      <c r="F75" s="47" t="s">
         <v>32</v>
       </c>
       <c r="G75" s="17"/>
@@ -10074,9 +10074,9 @@
       <c r="C76" s="3">
         <v>0.15</v>
       </c>
-      <c r="D76" s="49"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="49"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="49"/>
+      <c r="F76" s="47"/>
       <c r="G76" s="17"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -10165,13 +10165,13 @@
       <c r="C85" s="3">
         <v>0.12</v>
       </c>
-      <c r="D85" s="49" t="s">
+      <c r="D85" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E85" s="47" t="s">
+      <c r="E85" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F85" s="49" t="s">
+      <c r="F85" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10183,9 +10183,9 @@
       <c r="C86" s="3">
         <v>0.12</v>
       </c>
-      <c r="D86" s="49"/>
-      <c r="E86" s="48"/>
-      <c r="F86" s="49"/>
+      <c r="D86" s="47"/>
+      <c r="E86" s="49"/>
+      <c r="F86" s="47"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
@@ -10274,13 +10274,13 @@
       <c r="C96" s="3">
         <v>0.12</v>
       </c>
-      <c r="D96" s="49" t="s">
+      <c r="D96" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E96" s="47" t="s">
+      <c r="E96" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F96" s="49" t="s">
+      <c r="F96" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10292,9 +10292,9 @@
       <c r="C97" s="3">
         <v>0.12</v>
       </c>
-      <c r="D97" s="49"/>
-      <c r="E97" s="48"/>
-      <c r="F97" s="49"/>
+      <c r="D97" s="47"/>
+      <c r="E97" s="49"/>
+      <c r="F97" s="47"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
@@ -10419,13 +10419,13 @@
       <c r="C107" s="3">
         <v>0.12</v>
       </c>
-      <c r="D107" s="49" t="s">
+      <c r="D107" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E107" s="47" t="s">
+      <c r="E107" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F107" s="49" t="s">
+      <c r="F107" s="47" t="s">
         <v>31</v>
       </c>
       <c r="I107" s="1"/>
@@ -10435,13 +10435,13 @@
       <c r="K107" s="3">
         <v>0.12</v>
       </c>
-      <c r="L107" s="49" t="s">
+      <c r="L107" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="M107" s="47" t="s">
+      <c r="M107" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="N107" s="49" t="s">
+      <c r="N107" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10453,9 +10453,9 @@
       <c r="C108" s="3">
         <v>0.12</v>
       </c>
-      <c r="D108" s="49"/>
-      <c r="E108" s="48"/>
-      <c r="F108" s="49"/>
+      <c r="D108" s="47"/>
+      <c r="E108" s="49"/>
+      <c r="F108" s="47"/>
       <c r="I108" s="1"/>
       <c r="J108" s="2" t="s">
         <v>10</v>
@@ -10463,9 +10463,9 @@
       <c r="K108" s="3">
         <v>0.12</v>
       </c>
-      <c r="L108" s="49"/>
-      <c r="M108" s="48"/>
-      <c r="N108" s="49"/>
+      <c r="L108" s="47"/>
+      <c r="M108" s="49"/>
+      <c r="N108" s="47"/>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
@@ -10589,13 +10589,13 @@
       <c r="C118" s="3">
         <v>0.12</v>
       </c>
-      <c r="D118" s="49" t="s">
+      <c r="D118" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E118" s="47" t="s">
+      <c r="E118" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F118" s="49" t="s">
+      <c r="F118" s="47" t="s">
         <v>31</v>
       </c>
       <c r="G118" s="17"/>
@@ -10608,9 +10608,9 @@
       <c r="C119" s="3">
         <v>0.12</v>
       </c>
-      <c r="D119" s="49"/>
-      <c r="E119" s="48"/>
-      <c r="F119" s="49"/>
+      <c r="D119" s="47"/>
+      <c r="E119" s="49"/>
+      <c r="F119" s="47"/>
       <c r="G119" s="17"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
@@ -10708,13 +10708,13 @@
       <c r="C129" s="3">
         <v>0.12</v>
       </c>
-      <c r="D129" s="49" t="s">
+      <c r="D129" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E129" s="47" t="s">
+      <c r="E129" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F129" s="49" t="s">
+      <c r="F129" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10726,9 +10726,9 @@
       <c r="C130" s="3">
         <v>0.12</v>
       </c>
-      <c r="D130" s="49"/>
-      <c r="E130" s="48"/>
-      <c r="F130" s="49"/>
+      <c r="D130" s="47"/>
+      <c r="E130" s="49"/>
+      <c r="F130" s="47"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -10823,13 +10823,13 @@
       <c r="C140" s="3">
         <v>0.12</v>
       </c>
-      <c r="D140" s="49" t="s">
+      <c r="D140" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E140" s="47" t="s">
+      <c r="E140" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F140" s="49" t="s">
+      <c r="F140" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10841,9 +10841,9 @@
       <c r="C141" s="3">
         <v>0.12</v>
       </c>
-      <c r="D141" s="49"/>
-      <c r="E141" s="48"/>
-      <c r="F141" s="49"/>
+      <c r="D141" s="47"/>
+      <c r="E141" s="49"/>
+      <c r="F141" s="47"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
@@ -10935,13 +10935,13 @@
       <c r="C151" s="3">
         <v>0.12</v>
       </c>
-      <c r="D151" s="49" t="s">
+      <c r="D151" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E151" s="47" t="s">
+      <c r="E151" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F151" s="49" t="s">
+      <c r="F151" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10953,9 +10953,9 @@
       <c r="C152" s="3">
         <v>0.12</v>
       </c>
-      <c r="D152" s="49"/>
-      <c r="E152" s="48"/>
-      <c r="F152" s="49"/>
+      <c r="D152" s="47"/>
+      <c r="E152" s="49"/>
+      <c r="F152" s="47"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
@@ -11050,13 +11050,13 @@
       <c r="C162" s="3">
         <v>0.12</v>
       </c>
-      <c r="D162" s="49" t="s">
+      <c r="D162" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E162" s="47" t="s">
+      <c r="E162" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F162" s="49" t="s">
+      <c r="F162" s="47" t="s">
         <v>31</v>
       </c>
       <c r="G162" s="36"/>
@@ -11069,9 +11069,9 @@
       <c r="C163" s="3">
         <v>0.12</v>
       </c>
-      <c r="D163" s="49"/>
-      <c r="E163" s="48"/>
-      <c r="F163" s="49"/>
+      <c r="D163" s="47"/>
+      <c r="E163" s="49"/>
+      <c r="F163" s="47"/>
       <c r="G163" s="36"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -11168,13 +11168,13 @@
       <c r="C173" s="3">
         <v>0.12</v>
       </c>
-      <c r="D173" s="49" t="s">
+      <c r="D173" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E173" s="47" t="s">
+      <c r="E173" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F173" s="49" t="s">
+      <c r="F173" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11186,9 +11186,9 @@
       <c r="C174" s="3">
         <v>0.12</v>
       </c>
-      <c r="D174" s="49"/>
-      <c r="E174" s="48"/>
-      <c r="F174" s="49"/>
+      <c r="D174" s="47"/>
+      <c r="E174" s="49"/>
+      <c r="F174" s="47"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="8" t="s">
@@ -11283,13 +11283,13 @@
       <c r="C185" s="3">
         <v>0.12</v>
       </c>
-      <c r="D185" s="49" t="s">
+      <c r="D185" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E185" s="47" t="s">
+      <c r="E185" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F185" s="49" t="s">
+      <c r="F185" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11301,9 +11301,9 @@
       <c r="C186" s="3">
         <v>0.12</v>
       </c>
-      <c r="D186" s="49"/>
-      <c r="E186" s="48"/>
-      <c r="F186" s="49"/>
+      <c r="D186" s="47"/>
+      <c r="E186" s="49"/>
+      <c r="F186" s="47"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="8" t="s">
@@ -11396,13 +11396,13 @@
       <c r="C197" s="3">
         <v>0.12</v>
       </c>
-      <c r="D197" s="49" t="s">
+      <c r="D197" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E197" s="47" t="s">
+      <c r="E197" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F197" s="49" t="s">
+      <c r="F197" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11414,9 +11414,9 @@
       <c r="C198" s="3">
         <v>0.12</v>
       </c>
-      <c r="D198" s="49"/>
-      <c r="E198" s="48"/>
-      <c r="F198" s="49"/>
+      <c r="D198" s="47"/>
+      <c r="E198" s="49"/>
+      <c r="F198" s="47"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="8" t="s">
@@ -11514,13 +11514,13 @@
       <c r="C210" s="3">
         <v>0.12</v>
       </c>
-      <c r="D210" s="49" t="s">
+      <c r="D210" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E210" s="47" t="s">
+      <c r="E210" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F210" s="49" t="s">
+      <c r="F210" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11532,9 +11532,9 @@
       <c r="C211" s="3">
         <v>0.12</v>
       </c>
-      <c r="D211" s="49"/>
-      <c r="E211" s="48"/>
-      <c r="F211" s="49"/>
+      <c r="D211" s="47"/>
+      <c r="E211" s="49"/>
+      <c r="F211" s="47"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" s="8" t="s">
@@ -11624,13 +11624,13 @@
       <c r="C221" s="3">
         <v>0.12</v>
       </c>
-      <c r="D221" s="49" t="s">
+      <c r="D221" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E221" s="47" t="s">
+      <c r="E221" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F221" s="49" t="s">
+      <c r="F221" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11642,9 +11642,9 @@
       <c r="C222" s="3">
         <v>0.12</v>
       </c>
-      <c r="D222" s="49"/>
-      <c r="E222" s="48"/>
-      <c r="F222" s="49"/>
+      <c r="D222" s="47"/>
+      <c r="E222" s="49"/>
+      <c r="F222" s="47"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" s="8" t="s">
@@ -11734,13 +11734,13 @@
       <c r="C232" s="3">
         <v>0.12</v>
       </c>
-      <c r="D232" s="49" t="s">
+      <c r="D232" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E232" s="47" t="s">
+      <c r="E232" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F232" s="49" t="s">
+      <c r="F232" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11752,9 +11752,9 @@
       <c r="C233" s="3">
         <v>0.12</v>
       </c>
-      <c r="D233" s="49"/>
-      <c r="E233" s="48"/>
-      <c r="F233" s="49"/>
+      <c r="D233" s="47"/>
+      <c r="E233" s="49"/>
+      <c r="F233" s="47"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234" s="8" t="s">
@@ -11844,13 +11844,13 @@
       <c r="C243" s="3">
         <v>0.12</v>
       </c>
-      <c r="D243" s="49" t="s">
+      <c r="D243" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E243" s="47" t="s">
+      <c r="E243" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F243" s="49" t="s">
+      <c r="F243" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11862,9 +11862,9 @@
       <c r="C244" s="3">
         <v>0.12</v>
       </c>
-      <c r="D244" s="49"/>
-      <c r="E244" s="48"/>
-      <c r="F244" s="49"/>
+      <c r="D244" s="47"/>
+      <c r="E244" s="49"/>
+      <c r="F244" s="47"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" s="8" t="s">
@@ -11954,13 +11954,13 @@
       <c r="C254" s="3">
         <v>0.12</v>
       </c>
-      <c r="D254" s="49" t="s">
+      <c r="D254" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E254" s="47" t="s">
+      <c r="E254" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F254" s="49" t="s">
+      <c r="F254" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11972,9 +11972,9 @@
       <c r="C255" s="3">
         <v>0.12</v>
       </c>
-      <c r="D255" s="49"/>
-      <c r="E255" s="48"/>
-      <c r="F255" s="49"/>
+      <c r="D255" s="47"/>
+      <c r="E255" s="49"/>
+      <c r="F255" s="47"/>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256" s="8" t="s">
@@ -12017,21 +12017,49 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="D254:D255"/>
-    <mergeCell ref="E254:E255"/>
-    <mergeCell ref="F254:F255"/>
-    <mergeCell ref="D232:D233"/>
-    <mergeCell ref="E232:E233"/>
-    <mergeCell ref="F232:F233"/>
-    <mergeCell ref="D243:D244"/>
-    <mergeCell ref="E243:E244"/>
-    <mergeCell ref="F243:F244"/>
-    <mergeCell ref="D210:D211"/>
-    <mergeCell ref="E210:E211"/>
-    <mergeCell ref="F210:F211"/>
-    <mergeCell ref="D221:D222"/>
-    <mergeCell ref="E221:E222"/>
-    <mergeCell ref="F221:F222"/>
+    <mergeCell ref="E151:E152"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="D185:D186"/>
+    <mergeCell ref="E185:E186"/>
+    <mergeCell ref="F185:F186"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="D173:D174"/>
+    <mergeCell ref="E173:E174"/>
+    <mergeCell ref="F173:F174"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="F107:F108"/>
     <mergeCell ref="D197:D198"/>
     <mergeCell ref="E197:E198"/>
     <mergeCell ref="F197:F198"/>
@@ -12048,49 +12076,21 @@
     <mergeCell ref="E140:E141"/>
     <mergeCell ref="F140:F141"/>
     <mergeCell ref="D151:D152"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="F107:F108"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="E151:E152"/>
-    <mergeCell ref="F151:F152"/>
-    <mergeCell ref="D185:D186"/>
-    <mergeCell ref="E185:E186"/>
-    <mergeCell ref="F185:F186"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="D173:D174"/>
-    <mergeCell ref="E173:E174"/>
-    <mergeCell ref="F173:F174"/>
+    <mergeCell ref="D210:D211"/>
+    <mergeCell ref="E210:E211"/>
+    <mergeCell ref="F210:F211"/>
+    <mergeCell ref="D221:D222"/>
+    <mergeCell ref="E221:E222"/>
+    <mergeCell ref="F221:F222"/>
+    <mergeCell ref="D254:D255"/>
+    <mergeCell ref="E254:E255"/>
+    <mergeCell ref="F254:F255"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="E232:E233"/>
+    <mergeCell ref="F232:F233"/>
+    <mergeCell ref="D243:D244"/>
+    <mergeCell ref="E243:E244"/>
+    <mergeCell ref="F243:F244"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12219,13 +12219,13 @@
       <c r="C5" s="3">
         <v>0.12</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="47" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="1"/>
@@ -12235,13 +12235,13 @@
       <c r="K5" s="3">
         <v>0.12</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="L5" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="47" t="s">
+      <c r="M5" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="49" t="s">
+      <c r="N5" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12253,9 +12253,9 @@
       <c r="C6" s="3">
         <v>0.12</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="47"/>
       <c r="I6" s="1"/>
       <c r="J6" s="28" t="s">
         <v>10</v>
@@ -12263,9 +12263,9 @@
       <c r="K6" s="3">
         <v>0.12</v>
       </c>
-      <c r="L6" s="49"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="49"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -12425,13 +12425,13 @@
       <c r="C16" s="3">
         <v>0.12</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="47" t="s">
         <v>31</v>
       </c>
       <c r="I16" s="1"/>
@@ -12441,13 +12441,13 @@
       <c r="K16" s="3">
         <v>0.12</v>
       </c>
-      <c r="L16" s="49" t="s">
+      <c r="L16" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="47" t="s">
+      <c r="M16" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="49" t="s">
+      <c r="N16" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12459,9 +12459,9 @@
       <c r="C17" s="3">
         <v>0.12</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="47"/>
       <c r="I17" s="1"/>
       <c r="J17" s="28" t="s">
         <v>10</v>
@@ -12469,9 +12469,9 @@
       <c r="K17" s="3">
         <v>0.12</v>
       </c>
-      <c r="L17" s="49"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="47"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
@@ -12631,13 +12631,13 @@
       <c r="C27" s="3">
         <v>0.12</v>
       </c>
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="47" t="s">
+      <c r="E27" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="49" t="s">
+      <c r="F27" s="47" t="s">
         <v>31</v>
       </c>
       <c r="I27" s="1"/>
@@ -12647,13 +12647,13 @@
       <c r="K27" s="3">
         <v>0.12</v>
       </c>
-      <c r="L27" s="49" t="s">
+      <c r="L27" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="M27" s="47" t="s">
+      <c r="M27" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="N27" s="49" t="s">
+      <c r="N27" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12665,9 +12665,9 @@
       <c r="C28" s="3">
         <v>0.12</v>
       </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="49"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="47"/>
       <c r="I28" s="1"/>
       <c r="J28" s="28" t="s">
         <v>10</v>
@@ -12675,9 +12675,9 @@
       <c r="K28" s="3">
         <v>0.12</v>
       </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="49"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="47"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
@@ -12837,13 +12837,13 @@
       <c r="C38" s="3">
         <v>0.12</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="47" t="s">
+      <c r="E38" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="49" t="s">
+      <c r="F38" s="47" t="s">
         <v>31</v>
       </c>
       <c r="I38" s="1"/>
@@ -12853,13 +12853,13 @@
       <c r="K38" s="3">
         <v>0.12</v>
       </c>
-      <c r="L38" s="49" t="s">
+      <c r="L38" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="M38" s="47" t="s">
+      <c r="M38" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="N38" s="49" t="s">
+      <c r="N38" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12871,9 +12871,9 @@
       <c r="C39" s="3">
         <v>0.12</v>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="49"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="47"/>
       <c r="I39" s="1"/>
       <c r="J39" s="28" t="s">
         <v>10</v>
@@ -12881,9 +12881,9 @@
       <c r="K39" s="3">
         <v>0.12</v>
       </c>
-      <c r="L39" s="49"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="49"/>
+      <c r="L39" s="47"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="47"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
@@ -13019,13 +13019,13 @@
       <c r="C50" s="3">
         <v>0.12</v>
       </c>
-      <c r="D50" s="49" t="s">
+      <c r="D50" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="47" t="s">
+      <c r="E50" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="49" t="s">
+      <c r="F50" s="47" t="s">
         <v>31</v>
       </c>
       <c r="G50" s="39"/>
@@ -13041,9 +13041,9 @@
       <c r="C51" s="3">
         <v>0.12</v>
       </c>
-      <c r="D51" s="49"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="47"/>
       <c r="G51" s="39"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -13144,13 +13144,13 @@
       <c r="C61" s="3">
         <v>0.12</v>
       </c>
-      <c r="D61" s="49" t="s">
+      <c r="D61" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E61" s="47" t="s">
+      <c r="E61" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="49" t="s">
+      <c r="F61" s="47" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13162,9 +13162,9 @@
       <c r="C62" s="3">
         <v>0.12</v>
       </c>
-      <c r="D62" s="49"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="49"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="47"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
@@ -13209,22 +13209,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="N27:N28"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="E50:E51"/>
     <mergeCell ref="F50:F51"/>
@@ -13241,6 +13225,22 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13250,8 +13250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13281,6 +13281,9 @@
       </c>
       <c r="B2" s="27" t="s">
         <v>106</v>
+      </c>
+      <c r="E2">
+        <v>744</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -14232,7 +14235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more results are added
</commit_message>
<xml_diff>
--- a/New Analysis.xlsx
+++ b/New Analysis.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="154">
   <si>
     <t>Doc Name</t>
   </si>
@@ -753,6 +753,48 @@
   <si>
     <t>Shuffle = True</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>70 IPS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, 1 hidden, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>250</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nodes, OP 14</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1007,7 +1049,7 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1113,13 +1155,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,24 +1187,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1159,8 +1205,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9502,10 +9547,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="56"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -9554,13 +9599,13 @@
       <c r="C5" s="3">
         <v>0.15</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9572,9 +9617,9 @@
       <c r="C6" s="3">
         <v>0.15</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -9655,13 +9700,13 @@
       <c r="C15" s="3">
         <v>0.15</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9673,9 +9718,9 @@
       <c r="C16" s="3">
         <v>0.15</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
@@ -9756,13 +9801,13 @@
       <c r="C25" s="3">
         <v>0.12</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="49" t="s">
+      <c r="F25" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9774,9 +9819,9 @@
       <c r="C26" s="3">
         <v>0.12</v>
       </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="53"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
@@ -9863,7 +9908,7 @@
       <c r="E35" s="10">
         <v>49630</v>
       </c>
-      <c r="F35" s="49" t="s">
+      <c r="F35" s="53" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9881,7 +9926,7 @@
       <c r="E36" s="10">
         <v>49479</v>
       </c>
-      <c r="F36" s="49"/>
+      <c r="F36" s="53"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
@@ -9962,13 +10007,13 @@
       <c r="C45" s="3">
         <v>0.15</v>
       </c>
-      <c r="D45" s="49" t="s">
+      <c r="D45" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="47" t="s">
+      <c r="E45" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="49" t="s">
+      <c r="F45" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9980,9 +10025,9 @@
       <c r="C46" s="3">
         <v>0.15</v>
       </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="49"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="53"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
@@ -10063,13 +10108,13 @@
       <c r="C55" s="3">
         <v>0.15</v>
       </c>
-      <c r="D55" s="49" t="s">
+      <c r="D55" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="47" t="s">
+      <c r="E55" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="49" t="s">
+      <c r="F55" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10081,9 +10126,9 @@
       <c r="C56" s="3">
         <v>0.15</v>
       </c>
-      <c r="D56" s="49"/>
-      <c r="E56" s="48"/>
-      <c r="F56" s="49"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="53"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
@@ -10167,13 +10212,13 @@
       <c r="C65" s="3">
         <v>0.15</v>
       </c>
-      <c r="D65" s="49" t="s">
+      <c r="D65" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="47" t="s">
+      <c r="E65" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="49" t="s">
+      <c r="F65" s="53" t="s">
         <v>32</v>
       </c>
       <c r="G65" s="17"/>
@@ -10186,9 +10231,9 @@
       <c r="C66" s="3">
         <v>0.15</v>
       </c>
-      <c r="D66" s="49"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="49"/>
+      <c r="D66" s="53"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="53"/>
       <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -10280,13 +10325,13 @@
       <c r="C75" s="3">
         <v>0.15</v>
       </c>
-      <c r="D75" s="49" t="s">
+      <c r="D75" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="47" t="s">
+      <c r="E75" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F75" s="49" t="s">
+      <c r="F75" s="53" t="s">
         <v>32</v>
       </c>
       <c r="G75" s="17"/>
@@ -10299,9 +10344,9 @@
       <c r="C76" s="3">
         <v>0.15</v>
       </c>
-      <c r="D76" s="49"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="49"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="53"/>
       <c r="G76" s="17"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -10390,13 +10435,13 @@
       <c r="C85" s="3">
         <v>0.12</v>
       </c>
-      <c r="D85" s="49" t="s">
+      <c r="D85" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E85" s="47" t="s">
+      <c r="E85" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F85" s="49" t="s">
+      <c r="F85" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10408,9 +10453,9 @@
       <c r="C86" s="3">
         <v>0.12</v>
       </c>
-      <c r="D86" s="49"/>
-      <c r="E86" s="48"/>
-      <c r="F86" s="49"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="53"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
@@ -10499,13 +10544,13 @@
       <c r="C96" s="3">
         <v>0.12</v>
       </c>
-      <c r="D96" s="49" t="s">
+      <c r="D96" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E96" s="47" t="s">
+      <c r="E96" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F96" s="49" t="s">
+      <c r="F96" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10517,9 +10562,9 @@
       <c r="C97" s="3">
         <v>0.12</v>
       </c>
-      <c r="D97" s="49"/>
-      <c r="E97" s="48"/>
-      <c r="F97" s="49"/>
+      <c r="D97" s="53"/>
+      <c r="E97" s="55"/>
+      <c r="F97" s="53"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
@@ -10644,13 +10689,13 @@
       <c r="C107" s="3">
         <v>0.12</v>
       </c>
-      <c r="D107" s="49" t="s">
+      <c r="D107" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E107" s="47" t="s">
+      <c r="E107" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F107" s="49" t="s">
+      <c r="F107" s="53" t="s">
         <v>31</v>
       </c>
       <c r="I107" s="1"/>
@@ -10660,13 +10705,13 @@
       <c r="K107" s="3">
         <v>0.12</v>
       </c>
-      <c r="L107" s="49" t="s">
+      <c r="L107" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="M107" s="47" t="s">
+      <c r="M107" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="N107" s="49" t="s">
+      <c r="N107" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10678,9 +10723,9 @@
       <c r="C108" s="3">
         <v>0.12</v>
       </c>
-      <c r="D108" s="49"/>
-      <c r="E108" s="48"/>
-      <c r="F108" s="49"/>
+      <c r="D108" s="53"/>
+      <c r="E108" s="55"/>
+      <c r="F108" s="53"/>
       <c r="I108" s="1"/>
       <c r="J108" s="2" t="s">
         <v>10</v>
@@ -10688,9 +10733,9 @@
       <c r="K108" s="3">
         <v>0.12</v>
       </c>
-      <c r="L108" s="49"/>
-      <c r="M108" s="48"/>
-      <c r="N108" s="49"/>
+      <c r="L108" s="53"/>
+      <c r="M108" s="55"/>
+      <c r="N108" s="53"/>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
@@ -10814,13 +10859,13 @@
       <c r="C118" s="3">
         <v>0.12</v>
       </c>
-      <c r="D118" s="49" t="s">
+      <c r="D118" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E118" s="47" t="s">
+      <c r="E118" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F118" s="49" t="s">
+      <c r="F118" s="53" t="s">
         <v>31</v>
       </c>
       <c r="G118" s="17"/>
@@ -10833,9 +10878,9 @@
       <c r="C119" s="3">
         <v>0.12</v>
       </c>
-      <c r="D119" s="49"/>
-      <c r="E119" s="48"/>
-      <c r="F119" s="49"/>
+      <c r="D119" s="53"/>
+      <c r="E119" s="55"/>
+      <c r="F119" s="53"/>
       <c r="G119" s="17"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
@@ -10933,13 +10978,13 @@
       <c r="C129" s="3">
         <v>0.12</v>
       </c>
-      <c r="D129" s="49" t="s">
+      <c r="D129" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E129" s="47" t="s">
+      <c r="E129" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F129" s="49" t="s">
+      <c r="F129" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10951,9 +10996,9 @@
       <c r="C130" s="3">
         <v>0.12</v>
       </c>
-      <c r="D130" s="49"/>
-      <c r="E130" s="48"/>
-      <c r="F130" s="49"/>
+      <c r="D130" s="53"/>
+      <c r="E130" s="55"/>
+      <c r="F130" s="53"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -11048,13 +11093,13 @@
       <c r="C140" s="3">
         <v>0.12</v>
       </c>
-      <c r="D140" s="49" t="s">
+      <c r="D140" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E140" s="47" t="s">
+      <c r="E140" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F140" s="49" t="s">
+      <c r="F140" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11066,9 +11111,9 @@
       <c r="C141" s="3">
         <v>0.12</v>
       </c>
-      <c r="D141" s="49"/>
-      <c r="E141" s="48"/>
-      <c r="F141" s="49"/>
+      <c r="D141" s="53"/>
+      <c r="E141" s="55"/>
+      <c r="F141" s="53"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
@@ -11160,13 +11205,13 @@
       <c r="C151" s="3">
         <v>0.12</v>
       </c>
-      <c r="D151" s="49" t="s">
+      <c r="D151" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E151" s="47" t="s">
+      <c r="E151" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F151" s="49" t="s">
+      <c r="F151" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11178,9 +11223,9 @@
       <c r="C152" s="3">
         <v>0.12</v>
       </c>
-      <c r="D152" s="49"/>
-      <c r="E152" s="48"/>
-      <c r="F152" s="49"/>
+      <c r="D152" s="53"/>
+      <c r="E152" s="55"/>
+      <c r="F152" s="53"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
@@ -11275,13 +11320,13 @@
       <c r="C162" s="3">
         <v>0.12</v>
       </c>
-      <c r="D162" s="49" t="s">
+      <c r="D162" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E162" s="47" t="s">
+      <c r="E162" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F162" s="49" t="s">
+      <c r="F162" s="53" t="s">
         <v>31</v>
       </c>
       <c r="G162" s="36"/>
@@ -11294,9 +11339,9 @@
       <c r="C163" s="3">
         <v>0.12</v>
       </c>
-      <c r="D163" s="49"/>
-      <c r="E163" s="48"/>
-      <c r="F163" s="49"/>
+      <c r="D163" s="53"/>
+      <c r="E163" s="55"/>
+      <c r="F163" s="53"/>
       <c r="G163" s="36"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -11393,13 +11438,13 @@
       <c r="C173" s="3">
         <v>0.12</v>
       </c>
-      <c r="D173" s="49" t="s">
+      <c r="D173" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E173" s="47" t="s">
+      <c r="E173" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F173" s="49" t="s">
+      <c r="F173" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11411,9 +11456,9 @@
       <c r="C174" s="3">
         <v>0.12</v>
       </c>
-      <c r="D174" s="49"/>
-      <c r="E174" s="48"/>
-      <c r="F174" s="49"/>
+      <c r="D174" s="53"/>
+      <c r="E174" s="55"/>
+      <c r="F174" s="53"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="8" t="s">
@@ -11508,13 +11553,13 @@
       <c r="C185" s="3">
         <v>0.12</v>
       </c>
-      <c r="D185" s="49" t="s">
+      <c r="D185" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E185" s="47" t="s">
+      <c r="E185" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F185" s="49" t="s">
+      <c r="F185" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11526,9 +11571,9 @@
       <c r="C186" s="3">
         <v>0.12</v>
       </c>
-      <c r="D186" s="49"/>
-      <c r="E186" s="48"/>
-      <c r="F186" s="49"/>
+      <c r="D186" s="53"/>
+      <c r="E186" s="55"/>
+      <c r="F186" s="53"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="8" t="s">
@@ -11621,13 +11666,13 @@
       <c r="C197" s="3">
         <v>0.12</v>
       </c>
-      <c r="D197" s="49" t="s">
+      <c r="D197" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E197" s="47" t="s">
+      <c r="E197" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F197" s="49" t="s">
+      <c r="F197" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11639,9 +11684,9 @@
       <c r="C198" s="3">
         <v>0.12</v>
       </c>
-      <c r="D198" s="49"/>
-      <c r="E198" s="48"/>
-      <c r="F198" s="49"/>
+      <c r="D198" s="53"/>
+      <c r="E198" s="55"/>
+      <c r="F198" s="53"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="8" t="s">
@@ -11739,13 +11784,13 @@
       <c r="C210" s="3">
         <v>0.12</v>
       </c>
-      <c r="D210" s="49" t="s">
+      <c r="D210" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E210" s="47" t="s">
+      <c r="E210" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F210" s="49" t="s">
+      <c r="F210" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11757,9 +11802,9 @@
       <c r="C211" s="3">
         <v>0.12</v>
       </c>
-      <c r="D211" s="49"/>
-      <c r="E211" s="48"/>
-      <c r="F211" s="49"/>
+      <c r="D211" s="53"/>
+      <c r="E211" s="55"/>
+      <c r="F211" s="53"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" s="8" t="s">
@@ -11849,13 +11894,13 @@
       <c r="C221" s="3">
         <v>0.12</v>
       </c>
-      <c r="D221" s="49" t="s">
+      <c r="D221" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E221" s="47" t="s">
+      <c r="E221" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F221" s="49" t="s">
+      <c r="F221" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11867,9 +11912,9 @@
       <c r="C222" s="3">
         <v>0.12</v>
       </c>
-      <c r="D222" s="49"/>
-      <c r="E222" s="48"/>
-      <c r="F222" s="49"/>
+      <c r="D222" s="53"/>
+      <c r="E222" s="55"/>
+      <c r="F222" s="53"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" s="8" t="s">
@@ -11959,13 +12004,13 @@
       <c r="C232" s="3">
         <v>0.12</v>
       </c>
-      <c r="D232" s="49" t="s">
+      <c r="D232" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E232" s="47" t="s">
+      <c r="E232" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F232" s="49" t="s">
+      <c r="F232" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11977,9 +12022,9 @@
       <c r="C233" s="3">
         <v>0.12</v>
       </c>
-      <c r="D233" s="49"/>
-      <c r="E233" s="48"/>
-      <c r="F233" s="49"/>
+      <c r="D233" s="53"/>
+      <c r="E233" s="55"/>
+      <c r="F233" s="53"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234" s="8" t="s">
@@ -12069,13 +12114,13 @@
       <c r="C243" s="3">
         <v>0.12</v>
       </c>
-      <c r="D243" s="49" t="s">
+      <c r="D243" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E243" s="47" t="s">
+      <c r="E243" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F243" s="49" t="s">
+      <c r="F243" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12087,9 +12132,9 @@
       <c r="C244" s="3">
         <v>0.12</v>
       </c>
-      <c r="D244" s="49"/>
-      <c r="E244" s="48"/>
-      <c r="F244" s="49"/>
+      <c r="D244" s="53"/>
+      <c r="E244" s="55"/>
+      <c r="F244" s="53"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" s="8" t="s">
@@ -12179,13 +12224,13 @@
       <c r="C254" s="3">
         <v>0.12</v>
       </c>
-      <c r="D254" s="49" t="s">
+      <c r="D254" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E254" s="47" t="s">
+      <c r="E254" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F254" s="49" t="s">
+      <c r="F254" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12197,9 +12242,9 @@
       <c r="C255" s="3">
         <v>0.12</v>
       </c>
-      <c r="D255" s="49"/>
-      <c r="E255" s="48"/>
-      <c r="F255" s="49"/>
+      <c r="D255" s="53"/>
+      <c r="E255" s="55"/>
+      <c r="F255" s="53"/>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256" s="8" t="s">
@@ -12242,21 +12287,49 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="D254:D255"/>
-    <mergeCell ref="E254:E255"/>
-    <mergeCell ref="F254:F255"/>
-    <mergeCell ref="D232:D233"/>
-    <mergeCell ref="E232:E233"/>
-    <mergeCell ref="F232:F233"/>
-    <mergeCell ref="D243:D244"/>
-    <mergeCell ref="E243:E244"/>
-    <mergeCell ref="F243:F244"/>
-    <mergeCell ref="D210:D211"/>
-    <mergeCell ref="E210:E211"/>
-    <mergeCell ref="F210:F211"/>
-    <mergeCell ref="D221:D222"/>
-    <mergeCell ref="E221:E222"/>
-    <mergeCell ref="F221:F222"/>
+    <mergeCell ref="E151:E152"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="D185:D186"/>
+    <mergeCell ref="E185:E186"/>
+    <mergeCell ref="F185:F186"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="D173:D174"/>
+    <mergeCell ref="E173:E174"/>
+    <mergeCell ref="F173:F174"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="F107:F108"/>
     <mergeCell ref="D197:D198"/>
     <mergeCell ref="E197:E198"/>
     <mergeCell ref="F197:F198"/>
@@ -12273,49 +12346,21 @@
     <mergeCell ref="E140:E141"/>
     <mergeCell ref="F140:F141"/>
     <mergeCell ref="D151:D152"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="F107:F108"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="E151:E152"/>
-    <mergeCell ref="F151:F152"/>
-    <mergeCell ref="D185:D186"/>
-    <mergeCell ref="E185:E186"/>
-    <mergeCell ref="F185:F186"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="D173:D174"/>
-    <mergeCell ref="E173:E174"/>
-    <mergeCell ref="F173:F174"/>
+    <mergeCell ref="D210:D211"/>
+    <mergeCell ref="E210:E211"/>
+    <mergeCell ref="F210:F211"/>
+    <mergeCell ref="D221:D222"/>
+    <mergeCell ref="E221:E222"/>
+    <mergeCell ref="F221:F222"/>
+    <mergeCell ref="D254:D255"/>
+    <mergeCell ref="E254:E255"/>
+    <mergeCell ref="F254:F255"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="E232:E233"/>
+    <mergeCell ref="F232:F233"/>
+    <mergeCell ref="D243:D244"/>
+    <mergeCell ref="E243:E244"/>
+    <mergeCell ref="F243:F244"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12347,22 +12392,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="I1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="I1" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
@@ -12444,13 +12489,13 @@
       <c r="C5" s="3">
         <v>0.12</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="53" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="1"/>
@@ -12460,13 +12505,13 @@
       <c r="K5" s="3">
         <v>0.12</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="L5" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="47" t="s">
+      <c r="M5" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="49" t="s">
+      <c r="N5" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12478,9 +12523,9 @@
       <c r="C6" s="3">
         <v>0.12</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="53"/>
       <c r="I6" s="1"/>
       <c r="J6" s="28" t="s">
         <v>10</v>
@@ -12488,9 +12533,9 @@
       <c r="K6" s="3">
         <v>0.12</v>
       </c>
-      <c r="L6" s="49"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="49"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="53"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -12650,13 +12695,13 @@
       <c r="C16" s="3">
         <v>0.12</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="53" t="s">
         <v>31</v>
       </c>
       <c r="I16" s="1"/>
@@ -12666,13 +12711,13 @@
       <c r="K16" s="3">
         <v>0.12</v>
       </c>
-      <c r="L16" s="49" t="s">
+      <c r="L16" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="47" t="s">
+      <c r="M16" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="49" t="s">
+      <c r="N16" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12684,9 +12729,9 @@
       <c r="C17" s="3">
         <v>0.12</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="53"/>
       <c r="I17" s="1"/>
       <c r="J17" s="28" t="s">
         <v>10</v>
@@ -12694,9 +12739,9 @@
       <c r="K17" s="3">
         <v>0.12</v>
       </c>
-      <c r="L17" s="49"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="53"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
@@ -12856,13 +12901,13 @@
       <c r="C27" s="3">
         <v>0.12</v>
       </c>
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="47" t="s">
+      <c r="E27" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="49" t="s">
+      <c r="F27" s="53" t="s">
         <v>31</v>
       </c>
       <c r="I27" s="1"/>
@@ -12872,13 +12917,13 @@
       <c r="K27" s="3">
         <v>0.12</v>
       </c>
-      <c r="L27" s="49" t="s">
+      <c r="L27" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="M27" s="47" t="s">
+      <c r="M27" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="N27" s="49" t="s">
+      <c r="N27" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12890,9 +12935,9 @@
       <c r="C28" s="3">
         <v>0.12</v>
       </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="49"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="53"/>
       <c r="I28" s="1"/>
       <c r="J28" s="28" t="s">
         <v>10</v>
@@ -12900,9 +12945,9 @@
       <c r="K28" s="3">
         <v>0.12</v>
       </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="49"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="53"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
@@ -13062,13 +13107,13 @@
       <c r="C38" s="3">
         <v>0.12</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="47" t="s">
+      <c r="E38" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="49" t="s">
+      <c r="F38" s="53" t="s">
         <v>31</v>
       </c>
       <c r="I38" s="1"/>
@@ -13078,13 +13123,13 @@
       <c r="K38" s="3">
         <v>0.12</v>
       </c>
-      <c r="L38" s="49" t="s">
+      <c r="L38" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="M38" s="47" t="s">
+      <c r="M38" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="N38" s="49" t="s">
+      <c r="N38" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13096,9 +13141,9 @@
       <c r="C39" s="3">
         <v>0.12</v>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="49"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="53"/>
       <c r="I39" s="1"/>
       <c r="J39" s="28" t="s">
         <v>10</v>
@@ -13106,9 +13151,9 @@
       <c r="K39" s="3">
         <v>0.12</v>
       </c>
-      <c r="L39" s="49"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="49"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="53"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
@@ -13244,13 +13289,13 @@
       <c r="C50" s="3">
         <v>0.12</v>
       </c>
-      <c r="D50" s="49" t="s">
+      <c r="D50" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="47" t="s">
+      <c r="E50" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="49" t="s">
+      <c r="F50" s="53" t="s">
         <v>31</v>
       </c>
       <c r="G50" s="39"/>
@@ -13266,9 +13311,9 @@
       <c r="C51" s="3">
         <v>0.12</v>
       </c>
-      <c r="D51" s="49"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="53"/>
       <c r="G51" s="39"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -13369,13 +13414,13 @@
       <c r="C61" s="3">
         <v>0.12</v>
       </c>
-      <c r="D61" s="49" t="s">
+      <c r="D61" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E61" s="47" t="s">
+      <c r="E61" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="49" t="s">
+      <c r="F61" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13387,9 +13432,9 @@
       <c r="C62" s="3">
         <v>0.12</v>
       </c>
-      <c r="D62" s="49"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="49"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="53"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
@@ -13434,22 +13479,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="N27:N28"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="E50:E51"/>
     <mergeCell ref="F50:F51"/>
@@ -13466,6 +13495,22 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14230,16 +14275,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="I1" s="52" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="I1" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
@@ -14384,12 +14429,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="35" t="s">
@@ -14841,12 +14886,12 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1:T21"/>
+      <selection pane="bottomLeft" activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14872,33 +14917,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="62"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
       <c r="L1" s="1" t="s">
         <v>141</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
       <c r="U1" s="1" t="s">
         <v>141</v>
       </c>
@@ -14907,10 +14952,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="56">
+      <c r="B2" s="50">
         <v>30</v>
       </c>
       <c r="D2" s="1">
@@ -15000,50 +15045,50 @@
         <v>4</v>
       </c>
       <c r="B4" s="29"/>
-      <c r="C4" s="58">
+      <c r="C4" s="59">
         <v>11.41</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="53">
         <v>747</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="54">
         <v>37753</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="53" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="29"/>
-      <c r="K4" s="58">
+      <c r="K4" s="59">
         <f>(M4/M2)*100</f>
         <v>11.833364075365353</v>
       </c>
-      <c r="L4" s="49">
+      <c r="L4" s="53">
         <v>747</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="54">
         <v>39134</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="53" t="s">
         <v>31</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="S4" s="29"/>
-      <c r="T4" s="58">
+      <c r="T4" s="59">
         <f>(V4/V2)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U4" s="49">
+      <c r="U4" s="53">
         <v>747</v>
       </c>
-      <c r="V4" s="47">
+      <c r="V4" s="54">
         <v>49060</v>
       </c>
-      <c r="W4" s="49" t="s">
+      <c r="W4" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -15054,30 +15099,30 @@
       <c r="B5" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="53"/>
       <c r="I5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="K5" s="59"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="49"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="53"/>
       <c r="R5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="S5" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="T5" s="59"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="48"/>
-      <c r="W5" s="49"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="53"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
@@ -15149,7 +15194,7 @@
       <c r="A9" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="53" t="b">
+      <c r="B9" s="47" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="22">
@@ -15158,32 +15203,32 @@
       <c r="I9" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="J9" s="53" t="b">
+      <c r="J9" s="47" t="b">
         <v>1</v>
       </c>
       <c r="K9" s="22"/>
       <c r="R9" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="S9" s="53" t="b">
+      <c r="S9" s="47" t="b">
         <v>1</v>
       </c>
       <c r="T9" s="22"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="48" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="48" t="s">
         <v>142</v>
       </c>
       <c r="J10" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="R10" s="54" t="s">
+      <c r="R10" s="48" t="s">
         <v>142</v>
       </c>
       <c r="S10" s="33" t="s">
@@ -15194,9 +15239,9 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="R12" s="63"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
@@ -15220,11 +15265,11 @@
         <v>33</v>
       </c>
       <c r="T13" s="43"/>
-      <c r="U13" s="64">
+      <c r="U13" s="52">
         <f>SUM(U14:U16)</f>
         <v>6236</v>
       </c>
-      <c r="V13" s="64">
+      <c r="V13" s="52">
         <f>SUM(V14:V16)</f>
         <v>414742</v>
       </c>
@@ -15270,30 +15315,30 @@
       <c r="C15" s="28">
         <v>11.41</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="53">
         <v>747</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="54">
         <v>37753</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="53" t="s">
         <v>31</v>
       </c>
       <c r="R15" s="8" t="s">
         <v>4</v>
       </c>
       <c r="S15" s="29"/>
-      <c r="T15" s="58">
+      <c r="T15" s="59">
         <f>(V15/V13)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U15" s="49">
+      <c r="U15" s="53">
         <v>747</v>
       </c>
-      <c r="V15" s="47">
+      <c r="V15" s="54">
         <v>49060</v>
       </c>
-      <c r="W15" s="49" t="s">
+      <c r="W15" s="53" t="s">
         <v>31</v>
       </c>
     </row>
@@ -15307,19 +15352,19 @@
       <c r="C16" s="28">
         <v>11.41</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="53"/>
       <c r="R16" s="13" t="s">
         <v>12</v>
       </c>
       <c r="S16" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="T16" s="59"/>
-      <c r="U16" s="49"/>
-      <c r="V16" s="48"/>
-      <c r="W16" s="49"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="53"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
@@ -15373,7 +15418,7 @@
       <c r="A20" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="53" t="b">
+      <c r="B20" s="47" t="b">
         <v>1</v>
       </c>
       <c r="C20" s="22">
@@ -15382,19 +15427,19 @@
       <c r="R20" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="S20" s="53" t="b">
+      <c r="S20" s="47" t="b">
         <v>1</v>
       </c>
       <c r="T20" s="22"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="48" t="s">
         <v>142</v>
       </c>
       <c r="B21" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="R21" s="54" t="s">
+      <c r="R21" s="48" t="s">
         <v>142</v>
       </c>
       <c r="S21" s="33" t="s">
@@ -15405,9 +15450,9 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="51"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
@@ -15419,11 +15464,11 @@
         <v>34</v>
       </c>
       <c r="T25" s="43"/>
-      <c r="U25" s="64">
+      <c r="U25" s="52">
         <f>SUM(U26:U28)</f>
         <v>6236</v>
       </c>
-      <c r="V25" s="64">
+      <c r="V25" s="52">
         <f>SUM(V26:V28)</f>
         <v>414742</v>
       </c>
@@ -15451,14 +15496,14 @@
         <v>4</v>
       </c>
       <c r="S27" s="29"/>
-      <c r="T27" s="58">
+      <c r="T27" s="59">
         <f>(V27/V25)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U27" s="49">
+      <c r="U27" s="53">
         <v>747</v>
       </c>
-      <c r="V27" s="47">
+      <c r="V27" s="54">
         <v>49060</v>
       </c>
     </row>
@@ -15469,9 +15514,9 @@
       <c r="S28" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="T28" s="59"/>
-      <c r="U28" s="49"/>
-      <c r="V28" s="48"/>
+      <c r="T28" s="60"/>
+      <c r="U28" s="53"/>
+      <c r="V28" s="55"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="R29" s="13" t="s">
@@ -15504,13 +15549,13 @@
       <c r="R32" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="S32" s="53" t="b">
+      <c r="S32" s="47" t="b">
         <v>1</v>
       </c>
       <c r="T32" s="22"/>
     </row>
-    <row r="33" spans="18:20" x14ac:dyDescent="0.3">
-      <c r="R33" s="54" t="s">
+    <row r="33" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R33" s="48" t="s">
         <v>142</v>
       </c>
       <c r="S33" s="33" t="s">
@@ -15520,20 +15565,123 @@
         <v>0.54520000000000002</v>
       </c>
     </row>
+    <row r="35" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R35" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S35" s="26">
+        <v>29</v>
+      </c>
+      <c r="T35" s="43"/>
+      <c r="U35" s="52">
+        <f>SUM(U36:U38)</f>
+        <v>6236</v>
+      </c>
+      <c r="V35" s="52">
+        <f>SUM(V36:V38)</f>
+        <v>330709</v>
+      </c>
+    </row>
+    <row r="36" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R36" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S36" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="T36" s="28">
+        <f>(V36/V35)*100</f>
+        <v>88.584223592342511</v>
+      </c>
+      <c r="U36" s="2">
+        <v>5489</v>
+      </c>
+      <c r="V36" s="2">
+        <v>292956</v>
+      </c>
+    </row>
+    <row r="37" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="S37" s="29"/>
+      <c r="T37" s="59">
+        <f>(V37/V35)*100</f>
+        <v>11.415776407657487</v>
+      </c>
+      <c r="U37" s="53">
+        <v>747</v>
+      </c>
+      <c r="V37" s="54">
+        <v>37753</v>
+      </c>
+    </row>
+    <row r="38" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R38" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="S38" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="T38" s="60"/>
+      <c r="U38" s="53"/>
+      <c r="V38" s="55"/>
+    </row>
+    <row r="39" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R39" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="S39" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="T39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R40" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="S40" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R41" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="S41" s="30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R42" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="S42" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="T42" s="22"/>
+    </row>
+    <row r="43" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R43" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="S43" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="T43" s="22">
+        <v>0.35649999999999998</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="T27:T28"/>
-    <mergeCell ref="U27:U28"/>
-    <mergeCell ref="V27:V28"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="W4:W5"/>
+  <mergeCells count="28">
+    <mergeCell ref="V37:V38"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="T37:T38"/>
+    <mergeCell ref="U37:U38"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
@@ -15544,9 +15692,18 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="T27:T28"/>
+    <mergeCell ref="U27:U28"/>
+    <mergeCell ref="V27:V28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
correct shadda mistake in atb3
</commit_message>
<xml_diff>
--- a/New Analysis.xlsx
+++ b/New Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6300" tabRatio="668" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6300" tabRatio="668" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="All Results" sheetId="1" r:id="rId1"/>
@@ -1369,13 +1369,13 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1393,6 +1393,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1404,9 +1407,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9799,13 +9799,13 @@
       <c r="C5" s="3">
         <v>0.15</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9817,9 +9817,9 @@
       <c r="C6" s="3">
         <v>0.15</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="64"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="66"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -9900,13 +9900,13 @@
       <c r="C15" s="3">
         <v>0.15</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="65" t="s">
+      <c r="E15" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="64" t="s">
+      <c r="F15" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9918,9 +9918,9 @@
       <c r="C16" s="3">
         <v>0.15</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="64"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
@@ -10001,13 +10001,13 @@
       <c r="C25" s="3">
         <v>0.12</v>
       </c>
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="65" t="s">
+      <c r="E25" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="64" t="s">
+      <c r="F25" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10019,9 +10019,9 @@
       <c r="C26" s="3">
         <v>0.12</v>
       </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="64"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
@@ -10108,7 +10108,7 @@
       <c r="E35" s="10">
         <v>49630</v>
       </c>
-      <c r="F35" s="64" t="s">
+      <c r="F35" s="66" t="s">
         <v>25</v>
       </c>
     </row>
@@ -10126,7 +10126,7 @@
       <c r="E36" s="10">
         <v>49479</v>
       </c>
-      <c r="F36" s="64"/>
+      <c r="F36" s="66"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
@@ -10207,13 +10207,13 @@
       <c r="C45" s="3">
         <v>0.15</v>
       </c>
-      <c r="D45" s="64" t="s">
+      <c r="D45" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="65" t="s">
+      <c r="E45" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="64" t="s">
+      <c r="F45" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10225,9 +10225,9 @@
       <c r="C46" s="3">
         <v>0.15</v>
       </c>
-      <c r="D46" s="64"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="64"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="66"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
@@ -10308,13 +10308,13 @@
       <c r="C55" s="3">
         <v>0.15</v>
       </c>
-      <c r="D55" s="64" t="s">
+      <c r="D55" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="65" t="s">
+      <c r="E55" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="64" t="s">
+      <c r="F55" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10326,9 +10326,9 @@
       <c r="C56" s="3">
         <v>0.15</v>
       </c>
-      <c r="D56" s="64"/>
-      <c r="E56" s="66"/>
-      <c r="F56" s="64"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="66"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
@@ -10412,13 +10412,13 @@
       <c r="C65" s="3">
         <v>0.15</v>
       </c>
-      <c r="D65" s="64" t="s">
+      <c r="D65" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="65" t="s">
+      <c r="E65" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="64" t="s">
+      <c r="F65" s="66" t="s">
         <v>32</v>
       </c>
       <c r="G65" s="17"/>
@@ -10431,9 +10431,9 @@
       <c r="C66" s="3">
         <v>0.15</v>
       </c>
-      <c r="D66" s="64"/>
-      <c r="E66" s="66"/>
-      <c r="F66" s="64"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="65"/>
+      <c r="F66" s="66"/>
       <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -10525,13 +10525,13 @@
       <c r="C75" s="3">
         <v>0.15</v>
       </c>
-      <c r="D75" s="64" t="s">
+      <c r="D75" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="65" t="s">
+      <c r="E75" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F75" s="64" t="s">
+      <c r="F75" s="66" t="s">
         <v>32</v>
       </c>
       <c r="G75" s="17"/>
@@ -10544,9 +10544,9 @@
       <c r="C76" s="3">
         <v>0.15</v>
       </c>
-      <c r="D76" s="64"/>
-      <c r="E76" s="66"/>
-      <c r="F76" s="64"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="66"/>
       <c r="G76" s="17"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -10635,13 +10635,13 @@
       <c r="C85" s="3">
         <v>0.12</v>
       </c>
-      <c r="D85" s="64" t="s">
+      <c r="D85" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E85" s="65" t="s">
+      <c r="E85" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F85" s="64" t="s">
+      <c r="F85" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10653,9 +10653,9 @@
       <c r="C86" s="3">
         <v>0.12</v>
       </c>
-      <c r="D86" s="64"/>
-      <c r="E86" s="66"/>
-      <c r="F86" s="64"/>
+      <c r="D86" s="66"/>
+      <c r="E86" s="65"/>
+      <c r="F86" s="66"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
@@ -10744,13 +10744,13 @@
       <c r="C96" s="3">
         <v>0.12</v>
       </c>
-      <c r="D96" s="64" t="s">
+      <c r="D96" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E96" s="65" t="s">
+      <c r="E96" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F96" s="64" t="s">
+      <c r="F96" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10762,9 +10762,9 @@
       <c r="C97" s="3">
         <v>0.12</v>
       </c>
-      <c r="D97" s="64"/>
-      <c r="E97" s="66"/>
-      <c r="F97" s="64"/>
+      <c r="D97" s="66"/>
+      <c r="E97" s="65"/>
+      <c r="F97" s="66"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
@@ -10889,13 +10889,13 @@
       <c r="C107" s="3">
         <v>0.12</v>
       </c>
-      <c r="D107" s="64" t="s">
+      <c r="D107" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E107" s="65" t="s">
+      <c r="E107" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F107" s="64" t="s">
+      <c r="F107" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I107" s="1"/>
@@ -10905,13 +10905,13 @@
       <c r="K107" s="3">
         <v>0.12</v>
       </c>
-      <c r="L107" s="64" t="s">
+      <c r="L107" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M107" s="65" t="s">
+      <c r="M107" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N107" s="64" t="s">
+      <c r="N107" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10923,9 +10923,9 @@
       <c r="C108" s="3">
         <v>0.12</v>
       </c>
-      <c r="D108" s="64"/>
-      <c r="E108" s="66"/>
-      <c r="F108" s="64"/>
+      <c r="D108" s="66"/>
+      <c r="E108" s="65"/>
+      <c r="F108" s="66"/>
       <c r="I108" s="1"/>
       <c r="J108" s="2" t="s">
         <v>10</v>
@@ -10933,9 +10933,9 @@
       <c r="K108" s="3">
         <v>0.12</v>
       </c>
-      <c r="L108" s="64"/>
-      <c r="M108" s="66"/>
-      <c r="N108" s="64"/>
+      <c r="L108" s="66"/>
+      <c r="M108" s="65"/>
+      <c r="N108" s="66"/>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
@@ -11059,13 +11059,13 @@
       <c r="C118" s="3">
         <v>0.12</v>
       </c>
-      <c r="D118" s="64" t="s">
+      <c r="D118" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E118" s="65" t="s">
+      <c r="E118" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F118" s="64" t="s">
+      <c r="F118" s="66" t="s">
         <v>31</v>
       </c>
       <c r="G118" s="17"/>
@@ -11078,9 +11078,9 @@
       <c r="C119" s="3">
         <v>0.12</v>
       </c>
-      <c r="D119" s="64"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="64"/>
+      <c r="D119" s="66"/>
+      <c r="E119" s="65"/>
+      <c r="F119" s="66"/>
       <c r="G119" s="17"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
@@ -11178,13 +11178,13 @@
       <c r="C129" s="3">
         <v>0.12</v>
       </c>
-      <c r="D129" s="64" t="s">
+      <c r="D129" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E129" s="65" t="s">
+      <c r="E129" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F129" s="64" t="s">
+      <c r="F129" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11196,9 +11196,9 @@
       <c r="C130" s="3">
         <v>0.12</v>
       </c>
-      <c r="D130" s="64"/>
-      <c r="E130" s="66"/>
-      <c r="F130" s="64"/>
+      <c r="D130" s="66"/>
+      <c r="E130" s="65"/>
+      <c r="F130" s="66"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -11293,13 +11293,13 @@
       <c r="C140" s="3">
         <v>0.12</v>
       </c>
-      <c r="D140" s="64" t="s">
+      <c r="D140" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E140" s="65" t="s">
+      <c r="E140" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F140" s="64" t="s">
+      <c r="F140" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11311,9 +11311,9 @@
       <c r="C141" s="3">
         <v>0.12</v>
       </c>
-      <c r="D141" s="64"/>
-      <c r="E141" s="66"/>
-      <c r="F141" s="64"/>
+      <c r="D141" s="66"/>
+      <c r="E141" s="65"/>
+      <c r="F141" s="66"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
@@ -11405,13 +11405,13 @@
       <c r="C151" s="3">
         <v>0.12</v>
       </c>
-      <c r="D151" s="64" t="s">
+      <c r="D151" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E151" s="65" t="s">
+      <c r="E151" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F151" s="64" t="s">
+      <c r="F151" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11423,9 +11423,9 @@
       <c r="C152" s="3">
         <v>0.12</v>
       </c>
-      <c r="D152" s="64"/>
-      <c r="E152" s="66"/>
-      <c r="F152" s="64"/>
+      <c r="D152" s="66"/>
+      <c r="E152" s="65"/>
+      <c r="F152" s="66"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
@@ -11520,13 +11520,13 @@
       <c r="C162" s="3">
         <v>0.12</v>
       </c>
-      <c r="D162" s="64" t="s">
+      <c r="D162" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E162" s="65" t="s">
+      <c r="E162" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F162" s="64" t="s">
+      <c r="F162" s="66" t="s">
         <v>31</v>
       </c>
       <c r="G162" s="36"/>
@@ -11539,9 +11539,9 @@
       <c r="C163" s="3">
         <v>0.12</v>
       </c>
-      <c r="D163" s="64"/>
-      <c r="E163" s="66"/>
-      <c r="F163" s="64"/>
+      <c r="D163" s="66"/>
+      <c r="E163" s="65"/>
+      <c r="F163" s="66"/>
       <c r="G163" s="36"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -11638,13 +11638,13 @@
       <c r="C173" s="3">
         <v>0.12</v>
       </c>
-      <c r="D173" s="64" t="s">
+      <c r="D173" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E173" s="65" t="s">
+      <c r="E173" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F173" s="64" t="s">
+      <c r="F173" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11656,9 +11656,9 @@
       <c r="C174" s="3">
         <v>0.12</v>
       </c>
-      <c r="D174" s="64"/>
-      <c r="E174" s="66"/>
-      <c r="F174" s="64"/>
+      <c r="D174" s="66"/>
+      <c r="E174" s="65"/>
+      <c r="F174" s="66"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="8" t="s">
@@ -11753,13 +11753,13 @@
       <c r="C185" s="3">
         <v>0.12</v>
       </c>
-      <c r="D185" s="64" t="s">
+      <c r="D185" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E185" s="65" t="s">
+      <c r="E185" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F185" s="64" t="s">
+      <c r="F185" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11771,9 +11771,9 @@
       <c r="C186" s="3">
         <v>0.12</v>
       </c>
-      <c r="D186" s="64"/>
-      <c r="E186" s="66"/>
-      <c r="F186" s="64"/>
+      <c r="D186" s="66"/>
+      <c r="E186" s="65"/>
+      <c r="F186" s="66"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="8" t="s">
@@ -11866,13 +11866,13 @@
       <c r="C197" s="3">
         <v>0.12</v>
       </c>
-      <c r="D197" s="64" t="s">
+      <c r="D197" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E197" s="65" t="s">
+      <c r="E197" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F197" s="64" t="s">
+      <c r="F197" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11884,9 +11884,9 @@
       <c r="C198" s="3">
         <v>0.12</v>
       </c>
-      <c r="D198" s="64"/>
-      <c r="E198" s="66"/>
-      <c r="F198" s="64"/>
+      <c r="D198" s="66"/>
+      <c r="E198" s="65"/>
+      <c r="F198" s="66"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="8" t="s">
@@ -11984,13 +11984,13 @@
       <c r="C210" s="3">
         <v>0.12</v>
       </c>
-      <c r="D210" s="64" t="s">
+      <c r="D210" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E210" s="65" t="s">
+      <c r="E210" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F210" s="64" t="s">
+      <c r="F210" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12002,9 +12002,9 @@
       <c r="C211" s="3">
         <v>0.12</v>
       </c>
-      <c r="D211" s="64"/>
-      <c r="E211" s="66"/>
-      <c r="F211" s="64"/>
+      <c r="D211" s="66"/>
+      <c r="E211" s="65"/>
+      <c r="F211" s="66"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" s="8" t="s">
@@ -12094,13 +12094,13 @@
       <c r="C221" s="3">
         <v>0.12</v>
       </c>
-      <c r="D221" s="64" t="s">
+      <c r="D221" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E221" s="65" t="s">
+      <c r="E221" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F221" s="64" t="s">
+      <c r="F221" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12112,9 +12112,9 @@
       <c r="C222" s="3">
         <v>0.12</v>
       </c>
-      <c r="D222" s="64"/>
-      <c r="E222" s="66"/>
-      <c r="F222" s="64"/>
+      <c r="D222" s="66"/>
+      <c r="E222" s="65"/>
+      <c r="F222" s="66"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" s="8" t="s">
@@ -12204,13 +12204,13 @@
       <c r="C232" s="3">
         <v>0.12</v>
       </c>
-      <c r="D232" s="64" t="s">
+      <c r="D232" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E232" s="65" t="s">
+      <c r="E232" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F232" s="64" t="s">
+      <c r="F232" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12222,9 +12222,9 @@
       <c r="C233" s="3">
         <v>0.12</v>
       </c>
-      <c r="D233" s="64"/>
-      <c r="E233" s="66"/>
-      <c r="F233" s="64"/>
+      <c r="D233" s="66"/>
+      <c r="E233" s="65"/>
+      <c r="F233" s="66"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234" s="8" t="s">
@@ -12314,13 +12314,13 @@
       <c r="C243" s="3">
         <v>0.12</v>
       </c>
-      <c r="D243" s="64" t="s">
+      <c r="D243" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E243" s="65" t="s">
+      <c r="E243" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F243" s="64" t="s">
+      <c r="F243" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12332,9 +12332,9 @@
       <c r="C244" s="3">
         <v>0.12</v>
       </c>
-      <c r="D244" s="64"/>
-      <c r="E244" s="66"/>
-      <c r="F244" s="64"/>
+      <c r="D244" s="66"/>
+      <c r="E244" s="65"/>
+      <c r="F244" s="66"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" s="8" t="s">
@@ -12424,13 +12424,13 @@
       <c r="C254" s="3">
         <v>0.12</v>
       </c>
-      <c r="D254" s="64" t="s">
+      <c r="D254" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E254" s="65" t="s">
+      <c r="E254" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F254" s="64" t="s">
+      <c r="F254" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12442,9 +12442,9 @@
       <c r="C255" s="3">
         <v>0.12</v>
       </c>
-      <c r="D255" s="64"/>
-      <c r="E255" s="66"/>
-      <c r="F255" s="64"/>
+      <c r="D255" s="66"/>
+      <c r="E255" s="65"/>
+      <c r="F255" s="66"/>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256" s="8" t="s">
@@ -12487,49 +12487,21 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="E151:E152"/>
-    <mergeCell ref="F151:F152"/>
-    <mergeCell ref="D185:D186"/>
-    <mergeCell ref="E185:E186"/>
-    <mergeCell ref="F185:F186"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="D173:D174"/>
-    <mergeCell ref="E173:E174"/>
-    <mergeCell ref="F173:F174"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="D254:D255"/>
+    <mergeCell ref="E254:E255"/>
+    <mergeCell ref="F254:F255"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="E232:E233"/>
+    <mergeCell ref="F232:F233"/>
+    <mergeCell ref="D243:D244"/>
+    <mergeCell ref="E243:E244"/>
+    <mergeCell ref="F243:F244"/>
+    <mergeCell ref="D210:D211"/>
+    <mergeCell ref="E210:E211"/>
+    <mergeCell ref="F210:F211"/>
+    <mergeCell ref="D221:D222"/>
+    <mergeCell ref="E221:E222"/>
+    <mergeCell ref="F221:F222"/>
     <mergeCell ref="D197:D198"/>
     <mergeCell ref="E197:E198"/>
     <mergeCell ref="F197:F198"/>
@@ -12546,21 +12518,49 @@
     <mergeCell ref="E140:E141"/>
     <mergeCell ref="F140:F141"/>
     <mergeCell ref="D151:D152"/>
-    <mergeCell ref="D210:D211"/>
-    <mergeCell ref="E210:E211"/>
-    <mergeCell ref="F210:F211"/>
-    <mergeCell ref="D221:D222"/>
-    <mergeCell ref="E221:E222"/>
-    <mergeCell ref="F221:F222"/>
-    <mergeCell ref="D254:D255"/>
-    <mergeCell ref="E254:E255"/>
-    <mergeCell ref="F254:F255"/>
-    <mergeCell ref="D232:D233"/>
-    <mergeCell ref="E232:E233"/>
-    <mergeCell ref="F232:F233"/>
-    <mergeCell ref="D243:D244"/>
-    <mergeCell ref="E243:E244"/>
-    <mergeCell ref="F243:F244"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="E151:E152"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="D185:D186"/>
+    <mergeCell ref="E185:E186"/>
+    <mergeCell ref="F185:F186"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="D173:D174"/>
+    <mergeCell ref="E173:E174"/>
+    <mergeCell ref="F173:F174"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12689,13 +12689,13 @@
       <c r="C5" s="3">
         <v>0.12</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="1"/>
@@ -12705,13 +12705,13 @@
       <c r="K5" s="3">
         <v>0.12</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="65" t="s">
+      <c r="M5" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="64" t="s">
+      <c r="N5" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12723,9 +12723,9 @@
       <c r="C6" s="3">
         <v>0.12</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="64"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="66"/>
       <c r="I6" s="1"/>
       <c r="J6" s="28" t="s">
         <v>10</v>
@@ -12733,9 +12733,9 @@
       <c r="K6" s="3">
         <v>0.12</v>
       </c>
-      <c r="L6" s="64"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="64"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="66"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -12895,13 +12895,13 @@
       <c r="C16" s="3">
         <v>0.12</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I16" s="1"/>
@@ -12911,13 +12911,13 @@
       <c r="K16" s="3">
         <v>0.12</v>
       </c>
-      <c r="L16" s="64" t="s">
+      <c r="L16" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="65" t="s">
+      <c r="M16" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="64" t="s">
+      <c r="N16" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12929,9 +12929,9 @@
       <c r="C17" s="3">
         <v>0.12</v>
       </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="64"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="66"/>
       <c r="I17" s="1"/>
       <c r="J17" s="28" t="s">
         <v>10</v>
@@ -12939,9 +12939,9 @@
       <c r="K17" s="3">
         <v>0.12</v>
       </c>
-      <c r="L17" s="64"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="64"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="65"/>
+      <c r="N17" s="66"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
@@ -13101,13 +13101,13 @@
       <c r="C27" s="3">
         <v>0.12</v>
       </c>
-      <c r="D27" s="64" t="s">
+      <c r="D27" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="65" t="s">
+      <c r="E27" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="64" t="s">
+      <c r="F27" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I27" s="1"/>
@@ -13117,13 +13117,13 @@
       <c r="K27" s="3">
         <v>0.12</v>
       </c>
-      <c r="L27" s="64" t="s">
+      <c r="L27" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M27" s="65" t="s">
+      <c r="M27" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N27" s="64" t="s">
+      <c r="N27" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13135,9 +13135,9 @@
       <c r="C28" s="3">
         <v>0.12</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="64"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
       <c r="I28" s="1"/>
       <c r="J28" s="28" t="s">
         <v>10</v>
@@ -13145,9 +13145,9 @@
       <c r="K28" s="3">
         <v>0.12</v>
       </c>
-      <c r="L28" s="64"/>
-      <c r="M28" s="66"/>
-      <c r="N28" s="64"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="66"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
@@ -13307,13 +13307,13 @@
       <c r="C38" s="3">
         <v>0.12</v>
       </c>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="65" t="s">
+      <c r="E38" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="64" t="s">
+      <c r="F38" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I38" s="1"/>
@@ -13323,13 +13323,13 @@
       <c r="K38" s="3">
         <v>0.12</v>
       </c>
-      <c r="L38" s="64" t="s">
+      <c r="L38" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M38" s="65" t="s">
+      <c r="M38" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N38" s="64" t="s">
+      <c r="N38" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13341,9 +13341,9 @@
       <c r="C39" s="3">
         <v>0.12</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="64"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="66"/>
       <c r="I39" s="1"/>
       <c r="J39" s="28" t="s">
         <v>10</v>
@@ -13351,9 +13351,9 @@
       <c r="K39" s="3">
         <v>0.12</v>
       </c>
-      <c r="L39" s="64"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="64"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="65"/>
+      <c r="N39" s="66"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
@@ -13489,13 +13489,13 @@
       <c r="C50" s="3">
         <v>0.12</v>
       </c>
-      <c r="D50" s="64" t="s">
+      <c r="D50" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="65" t="s">
+      <c r="E50" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="64" t="s">
+      <c r="F50" s="66" t="s">
         <v>31</v>
       </c>
       <c r="G50" s="39"/>
@@ -13511,9 +13511,9 @@
       <c r="C51" s="3">
         <v>0.12</v>
       </c>
-      <c r="D51" s="64"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="64"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="66"/>
       <c r="G51" s="39"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -13614,13 +13614,13 @@
       <c r="C61" s="3">
         <v>0.12</v>
       </c>
-      <c r="D61" s="64" t="s">
+      <c r="D61" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E61" s="65" t="s">
+      <c r="E61" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="64" t="s">
+      <c r="F61" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13632,9 +13632,9 @@
       <c r="C62" s="3">
         <v>0.12</v>
       </c>
-      <c r="D62" s="64"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="64"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="66"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
@@ -13679,6 +13679,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="N27:N28"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="E50:E51"/>
     <mergeCell ref="F50:F51"/>
@@ -13695,22 +13711,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13720,8 +13720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14450,7 +14450,7 @@
         <v>3893</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="21" t="s">
         <v>11</v>
       </c>
@@ -14458,7 +14458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>0</v>
       </c>
@@ -14466,7 +14466,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="8" t="s">
         <v>4</v>
       </c>
@@ -14475,7 +14475,7 @@
         <v>3.7183255528019514</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="8" t="s">
         <v>109</v>
       </c>
@@ -14484,7 +14484,7 @@
         <v>1.6103778840796878</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
         <v>12</v>
       </c>
@@ -14492,7 +14492,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="13" t="s">
         <v>22</v>
       </c>
@@ -14500,7 +14500,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="13" t="s">
         <v>24</v>
       </c>
@@ -14508,7 +14508,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="20" t="s">
         <v>42</v>
       </c>
@@ -14516,20 +14516,36 @@
         <v>47</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="40" t="s">
         <v>114</v>
       </c>
       <c r="B105" s="41">
         <v>7742</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <f>B105-358</f>
+        <v>7384</v>
+      </c>
+      <c r="E105">
+        <f>(D105/E1)*100</f>
+        <v>3.5463854148656182</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="40" t="s">
         <v>115</v>
       </c>
       <c r="B106" s="41">
         <v>3353</v>
+      </c>
+      <c r="D106">
+        <f>B106-358</f>
+        <v>2995</v>
+      </c>
+      <c r="E106">
+        <f>(D106/E1)*100</f>
+        <v>1.438437746143354</v>
       </c>
     </row>
   </sheetData>
@@ -15170,7 +15186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
@@ -15200,11 +15216,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
       <c r="D1" s="1" t="s">
         <v>141</v>
       </c>
@@ -15214,22 +15230,22 @@
       <c r="G1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="74"/>
-      <c r="K1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="76"/>
       <c r="L1" s="1" t="s">
         <v>141</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
       <c r="U1" s="1" t="s">
         <v>141</v>
       </c>
@@ -15349,13 +15365,13 @@
       <c r="C4" s="70">
         <v>11.41</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="66">
         <v>747</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="64">
         <v>37753</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="66" t="s">
         <v>31</v>
       </c>
       <c r="G4" t="s">
@@ -15369,13 +15385,13 @@
         <f>(M4/M2)*100</f>
         <v>11.833364075365353</v>
       </c>
-      <c r="L4" s="64">
+      <c r="L4" s="66">
         <v>747</v>
       </c>
-      <c r="M4" s="65">
+      <c r="M4" s="64">
         <v>39134</v>
       </c>
-      <c r="N4" s="64" t="s">
+      <c r="N4" s="66" t="s">
         <v>31</v>
       </c>
       <c r="R4" s="8" t="s">
@@ -15386,13 +15402,13 @@
         <f>(V4/V2)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U4" s="64">
+      <c r="U4" s="66">
         <v>747</v>
       </c>
-      <c r="V4" s="65">
+      <c r="V4" s="64">
         <v>49060</v>
       </c>
-      <c r="W4" s="64" t="s">
+      <c r="W4" s="66" t="s">
         <v>31</v>
       </c>
       <c r="X4" t="s">
@@ -15407,9 +15423,9 @@
         <v>108</v>
       </c>
       <c r="C5" s="71"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="64"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="66"/>
       <c r="G5" t="s">
         <v>155</v>
       </c>
@@ -15420,9 +15436,9 @@
         <v>108</v>
       </c>
       <c r="K5" s="71"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="64"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="66"/>
       <c r="R5" s="13" t="s">
         <v>12</v>
       </c>
@@ -15430,9 +15446,9 @@
         <v>108</v>
       </c>
       <c r="T5" s="71"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="64"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="66"/>
       <c r="X5" t="s">
         <v>155</v>
       </c>
@@ -15677,13 +15693,13 @@
       <c r="C15" s="28">
         <v>11.41</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="66">
         <v>747</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="64">
         <v>37753</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="72" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="54" t="s">
@@ -15697,13 +15713,13 @@
         <f>(V15/V13)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U15" s="64">
+      <c r="U15" s="66">
         <v>747</v>
       </c>
-      <c r="V15" s="65">
+      <c r="V15" s="64">
         <v>49060</v>
       </c>
-      <c r="W15" s="64" t="s">
+      <c r="W15" s="66" t="s">
         <v>31</v>
       </c>
       <c r="X15" t="s">
@@ -15720,9 +15736,9 @@
       <c r="C16" s="28">
         <v>11.41</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="76"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="72"/>
       <c r="G16" s="54" t="s">
         <v>156</v>
       </c>
@@ -15733,9 +15749,9 @@
         <v>108</v>
       </c>
       <c r="T16" s="71"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="66"/>
-      <c r="W16" s="64"/>
+      <c r="U16" s="66"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="66"/>
       <c r="X16" t="s">
         <v>155</v>
       </c>
@@ -15990,10 +16006,10 @@
         <f>(V27/V25)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U27" s="64">
+      <c r="U27" s="66">
         <v>747</v>
       </c>
-      <c r="V27" s="65">
+      <c r="V27" s="64">
         <v>49060</v>
       </c>
       <c r="X27" t="s">
@@ -16010,13 +16026,13 @@
       <c r="C28" s="28">
         <v>11.41</v>
       </c>
-      <c r="D28" s="64">
+      <c r="D28" s="66">
         <v>747</v>
       </c>
-      <c r="E28" s="65">
+      <c r="E28" s="64">
         <v>37753</v>
       </c>
-      <c r="F28" s="76" t="s">
+      <c r="F28" s="72" t="s">
         <v>31</v>
       </c>
       <c r="G28" s="58"/>
@@ -16027,8 +16043,8 @@
         <v>108</v>
       </c>
       <c r="T28" s="71"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="66"/>
+      <c r="U28" s="66"/>
+      <c r="V28" s="65"/>
       <c r="X28" t="s">
         <v>155</v>
       </c>
@@ -16043,9 +16059,9 @@
       <c r="C29" s="28">
         <v>11.41</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="76"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="72"/>
       <c r="G29" s="58"/>
       <c r="R29" s="13" t="s">
         <v>22</v>
@@ -16246,10 +16262,10 @@
         <f>(V37/V35)*100</f>
         <v>11.415776407657487</v>
       </c>
-      <c r="U37" s="64">
+      <c r="U37" s="66">
         <v>747</v>
       </c>
-      <c r="V37" s="65">
+      <c r="V37" s="64">
         <v>37753</v>
       </c>
       <c r="X37" t="s">
@@ -16263,8 +16279,8 @@
       </c>
       <c r="S38" s="30"/>
       <c r="T38" s="71"/>
-      <c r="U38" s="64"/>
-      <c r="V38" s="66"/>
+      <c r="U38" s="66"/>
+      <c r="V38" s="65"/>
       <c r="X38" t="s">
         <v>155</v>
       </c>
@@ -16333,13 +16349,13 @@
       <c r="C41" s="28">
         <v>11.41</v>
       </c>
-      <c r="D41" s="64">
+      <c r="D41" s="66">
         <v>747</v>
       </c>
-      <c r="E41" s="65">
+      <c r="E41" s="64">
         <v>37753</v>
       </c>
-      <c r="F41" s="76" t="s">
+      <c r="F41" s="72" t="s">
         <v>31</v>
       </c>
       <c r="G41" s="58"/>
@@ -16361,9 +16377,9 @@
       <c r="C42" s="28">
         <v>11.41</v>
       </c>
-      <c r="D42" s="64"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="76"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="72"/>
       <c r="G42" s="58"/>
       <c r="R42" s="13" t="s">
         <v>132</v>
@@ -16504,10 +16520,10 @@
         <f>(V48/V46)*100</f>
         <v>11.415776407657487</v>
       </c>
-      <c r="U48" s="64">
+      <c r="U48" s="66">
         <v>747</v>
       </c>
-      <c r="V48" s="65">
+      <c r="V48" s="64">
         <v>37753</v>
       </c>
     </row>
@@ -16532,8 +16548,8 @@
       </c>
       <c r="S49" s="30"/>
       <c r="T49" s="71"/>
-      <c r="U49" s="64"/>
-      <c r="V49" s="66"/>
+      <c r="U49" s="66"/>
+      <c r="V49" s="65"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C50" s="58"/>
@@ -16629,10 +16645,10 @@
         <f>(V58/V56)*100</f>
         <v>11.415776407657487</v>
       </c>
-      <c r="U58" s="64">
+      <c r="U58" s="66">
         <v>747</v>
       </c>
-      <c r="V58" s="65">
+      <c r="V58" s="64">
         <v>37753</v>
       </c>
     </row>
@@ -16642,8 +16658,8 @@
       </c>
       <c r="S59" s="30"/>
       <c r="T59" s="71"/>
-      <c r="U59" s="64"/>
-      <c r="V59" s="66"/>
+      <c r="U59" s="66"/>
+      <c r="V59" s="65"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="R60" s="13" t="s">
@@ -16689,15 +16705,25 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="V48:V49"/>
-    <mergeCell ref="T58:T59"/>
-    <mergeCell ref="U58:U59"/>
-    <mergeCell ref="V58:V59"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="T48:T49"/>
-    <mergeCell ref="U48:U49"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="T27:T28"/>
+    <mergeCell ref="U27:U28"/>
+    <mergeCell ref="V27:V28"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="V37:V38"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="E15:E16"/>
@@ -16710,25 +16736,15 @@
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="T27:T28"/>
-    <mergeCell ref="U27:U28"/>
-    <mergeCell ref="V27:V28"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="V48:V49"/>
+    <mergeCell ref="T58:T59"/>
+    <mergeCell ref="U58:U59"/>
+    <mergeCell ref="V58:V59"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="T48:T49"/>
+    <mergeCell ref="U48:U49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modify code to accept new labels encoding
</commit_message>
<xml_diff>
--- a/New Analysis.xlsx
+++ b/New Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6300" tabRatio="668" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6300" tabRatio="668" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="All Results" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="169">
   <si>
     <t>Doc Name</t>
   </si>
@@ -959,6 +959,31 @@
   <si>
     <t>39 IPS, 2 hidden, 250 nodes, OP 450</t>
   </si>
+  <si>
+    <r>
+      <t>39 IPS, 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hidden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 250 nodes, OP 49</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1228,7 +1253,7 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1369,13 +1394,13 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1393,6 +1418,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1405,8 +1433,8 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9727,7 +9755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N260"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A238" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C252" sqref="C252:F255"/>
     </sheetView>
   </sheetViews>
@@ -9799,13 +9827,13 @@
       <c r="C5" s="3">
         <v>0.15</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9817,9 +9845,9 @@
       <c r="C6" s="3">
         <v>0.15</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="64"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="66"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -9900,13 +9928,13 @@
       <c r="C15" s="3">
         <v>0.15</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="65" t="s">
+      <c r="E15" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="64" t="s">
+      <c r="F15" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9918,9 +9946,9 @@
       <c r="C16" s="3">
         <v>0.15</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="64"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
@@ -10001,13 +10029,13 @@
       <c r="C25" s="3">
         <v>0.12</v>
       </c>
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="65" t="s">
+      <c r="E25" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="64" t="s">
+      <c r="F25" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10019,9 +10047,9 @@
       <c r="C26" s="3">
         <v>0.12</v>
       </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="64"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
@@ -10108,7 +10136,7 @@
       <c r="E35" s="10">
         <v>49630</v>
       </c>
-      <c r="F35" s="64" t="s">
+      <c r="F35" s="66" t="s">
         <v>25</v>
       </c>
     </row>
@@ -10126,7 +10154,7 @@
       <c r="E36" s="10">
         <v>49479</v>
       </c>
-      <c r="F36" s="64"/>
+      <c r="F36" s="66"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
@@ -10207,13 +10235,13 @@
       <c r="C45" s="3">
         <v>0.15</v>
       </c>
-      <c r="D45" s="64" t="s">
+      <c r="D45" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="65" t="s">
+      <c r="E45" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="64" t="s">
+      <c r="F45" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10225,9 +10253,9 @@
       <c r="C46" s="3">
         <v>0.15</v>
       </c>
-      <c r="D46" s="64"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="64"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="66"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
@@ -10308,13 +10336,13 @@
       <c r="C55" s="3">
         <v>0.15</v>
       </c>
-      <c r="D55" s="64" t="s">
+      <c r="D55" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="65" t="s">
+      <c r="E55" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="64" t="s">
+      <c r="F55" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10326,9 +10354,9 @@
       <c r="C56" s="3">
         <v>0.15</v>
       </c>
-      <c r="D56" s="64"/>
-      <c r="E56" s="66"/>
-      <c r="F56" s="64"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="66"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
@@ -10412,13 +10440,13 @@
       <c r="C65" s="3">
         <v>0.15</v>
       </c>
-      <c r="D65" s="64" t="s">
+      <c r="D65" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="65" t="s">
+      <c r="E65" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="64" t="s">
+      <c r="F65" s="66" t="s">
         <v>32</v>
       </c>
       <c r="G65" s="17"/>
@@ -10431,9 +10459,9 @@
       <c r="C66" s="3">
         <v>0.15</v>
       </c>
-      <c r="D66" s="64"/>
-      <c r="E66" s="66"/>
-      <c r="F66" s="64"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="65"/>
+      <c r="F66" s="66"/>
       <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -10525,13 +10553,13 @@
       <c r="C75" s="3">
         <v>0.15</v>
       </c>
-      <c r="D75" s="64" t="s">
+      <c r="D75" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="65" t="s">
+      <c r="E75" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F75" s="64" t="s">
+      <c r="F75" s="66" t="s">
         <v>32</v>
       </c>
       <c r="G75" s="17"/>
@@ -10544,9 +10572,9 @@
       <c r="C76" s="3">
         <v>0.15</v>
       </c>
-      <c r="D76" s="64"/>
-      <c r="E76" s="66"/>
-      <c r="F76" s="64"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="66"/>
       <c r="G76" s="17"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -10635,13 +10663,13 @@
       <c r="C85" s="3">
         <v>0.12</v>
       </c>
-      <c r="D85" s="64" t="s">
+      <c r="D85" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E85" s="65" t="s">
+      <c r="E85" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F85" s="64" t="s">
+      <c r="F85" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10653,9 +10681,9 @@
       <c r="C86" s="3">
         <v>0.12</v>
       </c>
-      <c r="D86" s="64"/>
-      <c r="E86" s="66"/>
-      <c r="F86" s="64"/>
+      <c r="D86" s="66"/>
+      <c r="E86" s="65"/>
+      <c r="F86" s="66"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
@@ -10744,13 +10772,13 @@
       <c r="C96" s="3">
         <v>0.12</v>
       </c>
-      <c r="D96" s="64" t="s">
+      <c r="D96" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E96" s="65" t="s">
+      <c r="E96" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F96" s="64" t="s">
+      <c r="F96" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10762,9 +10790,9 @@
       <c r="C97" s="3">
         <v>0.12</v>
       </c>
-      <c r="D97" s="64"/>
-      <c r="E97" s="66"/>
-      <c r="F97" s="64"/>
+      <c r="D97" s="66"/>
+      <c r="E97" s="65"/>
+      <c r="F97" s="66"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
@@ -10889,13 +10917,13 @@
       <c r="C107" s="3">
         <v>0.12</v>
       </c>
-      <c r="D107" s="64" t="s">
+      <c r="D107" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E107" s="65" t="s">
+      <c r="E107" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F107" s="64" t="s">
+      <c r="F107" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I107" s="1"/>
@@ -10905,13 +10933,13 @@
       <c r="K107" s="3">
         <v>0.12</v>
       </c>
-      <c r="L107" s="64" t="s">
+      <c r="L107" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M107" s="65" t="s">
+      <c r="M107" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N107" s="64" t="s">
+      <c r="N107" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -10923,9 +10951,9 @@
       <c r="C108" s="3">
         <v>0.12</v>
       </c>
-      <c r="D108" s="64"/>
-      <c r="E108" s="66"/>
-      <c r="F108" s="64"/>
+      <c r="D108" s="66"/>
+      <c r="E108" s="65"/>
+      <c r="F108" s="66"/>
       <c r="I108" s="1"/>
       <c r="J108" s="2" t="s">
         <v>10</v>
@@ -10933,9 +10961,9 @@
       <c r="K108" s="3">
         <v>0.12</v>
       </c>
-      <c r="L108" s="64"/>
-      <c r="M108" s="66"/>
-      <c r="N108" s="64"/>
+      <c r="L108" s="66"/>
+      <c r="M108" s="65"/>
+      <c r="N108" s="66"/>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
@@ -11059,13 +11087,13 @@
       <c r="C118" s="3">
         <v>0.12</v>
       </c>
-      <c r="D118" s="64" t="s">
+      <c r="D118" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E118" s="65" t="s">
+      <c r="E118" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F118" s="64" t="s">
+      <c r="F118" s="66" t="s">
         <v>31</v>
       </c>
       <c r="G118" s="17"/>
@@ -11078,9 +11106,9 @@
       <c r="C119" s="3">
         <v>0.12</v>
       </c>
-      <c r="D119" s="64"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="64"/>
+      <c r="D119" s="66"/>
+      <c r="E119" s="65"/>
+      <c r="F119" s="66"/>
       <c r="G119" s="17"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
@@ -11178,13 +11206,13 @@
       <c r="C129" s="3">
         <v>0.12</v>
       </c>
-      <c r="D129" s="64" t="s">
+      <c r="D129" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E129" s="65" t="s">
+      <c r="E129" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F129" s="64" t="s">
+      <c r="F129" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11196,9 +11224,9 @@
       <c r="C130" s="3">
         <v>0.12</v>
       </c>
-      <c r="D130" s="64"/>
-      <c r="E130" s="66"/>
-      <c r="F130" s="64"/>
+      <c r="D130" s="66"/>
+      <c r="E130" s="65"/>
+      <c r="F130" s="66"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -11293,13 +11321,13 @@
       <c r="C140" s="3">
         <v>0.12</v>
       </c>
-      <c r="D140" s="64" t="s">
+      <c r="D140" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E140" s="65" t="s">
+      <c r="E140" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F140" s="64" t="s">
+      <c r="F140" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11311,9 +11339,9 @@
       <c r="C141" s="3">
         <v>0.12</v>
       </c>
-      <c r="D141" s="64"/>
-      <c r="E141" s="66"/>
-      <c r="F141" s="64"/>
+      <c r="D141" s="66"/>
+      <c r="E141" s="65"/>
+      <c r="F141" s="66"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
@@ -11405,13 +11433,13 @@
       <c r="C151" s="3">
         <v>0.12</v>
       </c>
-      <c r="D151" s="64" t="s">
+      <c r="D151" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E151" s="65" t="s">
+      <c r="E151" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F151" s="64" t="s">
+      <c r="F151" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11423,9 +11451,9 @@
       <c r="C152" s="3">
         <v>0.12</v>
       </c>
-      <c r="D152" s="64"/>
-      <c r="E152" s="66"/>
-      <c r="F152" s="64"/>
+      <c r="D152" s="66"/>
+      <c r="E152" s="65"/>
+      <c r="F152" s="66"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
@@ -11520,13 +11548,13 @@
       <c r="C162" s="3">
         <v>0.12</v>
       </c>
-      <c r="D162" s="64" t="s">
+      <c r="D162" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E162" s="65" t="s">
+      <c r="E162" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F162" s="64" t="s">
+      <c r="F162" s="66" t="s">
         <v>31</v>
       </c>
       <c r="G162" s="36"/>
@@ -11539,9 +11567,9 @@
       <c r="C163" s="3">
         <v>0.12</v>
       </c>
-      <c r="D163" s="64"/>
-      <c r="E163" s="66"/>
-      <c r="F163" s="64"/>
+      <c r="D163" s="66"/>
+      <c r="E163" s="65"/>
+      <c r="F163" s="66"/>
       <c r="G163" s="36"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -11638,13 +11666,13 @@
       <c r="C173" s="3">
         <v>0.12</v>
       </c>
-      <c r="D173" s="64" t="s">
+      <c r="D173" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E173" s="65" t="s">
+      <c r="E173" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F173" s="64" t="s">
+      <c r="F173" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11656,9 +11684,9 @@
       <c r="C174" s="3">
         <v>0.12</v>
       </c>
-      <c r="D174" s="64"/>
-      <c r="E174" s="66"/>
-      <c r="F174" s="64"/>
+      <c r="D174" s="66"/>
+      <c r="E174" s="65"/>
+      <c r="F174" s="66"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="8" t="s">
@@ -11753,13 +11781,13 @@
       <c r="C185" s="3">
         <v>0.12</v>
       </c>
-      <c r="D185" s="64" t="s">
+      <c r="D185" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E185" s="65" t="s">
+      <c r="E185" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F185" s="64" t="s">
+      <c r="F185" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11771,9 +11799,9 @@
       <c r="C186" s="3">
         <v>0.12</v>
       </c>
-      <c r="D186" s="64"/>
-      <c r="E186" s="66"/>
-      <c r="F186" s="64"/>
+      <c r="D186" s="66"/>
+      <c r="E186" s="65"/>
+      <c r="F186" s="66"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="8" t="s">
@@ -11866,13 +11894,13 @@
       <c r="C197" s="3">
         <v>0.12</v>
       </c>
-      <c r="D197" s="64" t="s">
+      <c r="D197" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E197" s="65" t="s">
+      <c r="E197" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F197" s="64" t="s">
+      <c r="F197" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11884,9 +11912,9 @@
       <c r="C198" s="3">
         <v>0.12</v>
       </c>
-      <c r="D198" s="64"/>
-      <c r="E198" s="66"/>
-      <c r="F198" s="64"/>
+      <c r="D198" s="66"/>
+      <c r="E198" s="65"/>
+      <c r="F198" s="66"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="8" t="s">
@@ -11984,13 +12012,13 @@
       <c r="C210" s="3">
         <v>0.12</v>
       </c>
-      <c r="D210" s="64" t="s">
+      <c r="D210" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E210" s="65" t="s">
+      <c r="E210" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F210" s="64" t="s">
+      <c r="F210" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12002,9 +12030,9 @@
       <c r="C211" s="3">
         <v>0.12</v>
       </c>
-      <c r="D211" s="64"/>
-      <c r="E211" s="66"/>
-      <c r="F211" s="64"/>
+      <c r="D211" s="66"/>
+      <c r="E211" s="65"/>
+      <c r="F211" s="66"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" s="8" t="s">
@@ -12094,13 +12122,13 @@
       <c r="C221" s="3">
         <v>0.12</v>
       </c>
-      <c r="D221" s="64" t="s">
+      <c r="D221" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E221" s="65" t="s">
+      <c r="E221" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F221" s="64" t="s">
+      <c r="F221" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12112,9 +12140,9 @@
       <c r="C222" s="3">
         <v>0.12</v>
       </c>
-      <c r="D222" s="64"/>
-      <c r="E222" s="66"/>
-      <c r="F222" s="64"/>
+      <c r="D222" s="66"/>
+      <c r="E222" s="65"/>
+      <c r="F222" s="66"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" s="8" t="s">
@@ -12204,13 +12232,13 @@
       <c r="C232" s="3">
         <v>0.12</v>
       </c>
-      <c r="D232" s="64" t="s">
+      <c r="D232" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E232" s="65" t="s">
+      <c r="E232" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F232" s="64" t="s">
+      <c r="F232" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12222,9 +12250,9 @@
       <c r="C233" s="3">
         <v>0.12</v>
       </c>
-      <c r="D233" s="64"/>
-      <c r="E233" s="66"/>
-      <c r="F233" s="64"/>
+      <c r="D233" s="66"/>
+      <c r="E233" s="65"/>
+      <c r="F233" s="66"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234" s="8" t="s">
@@ -12314,13 +12342,13 @@
       <c r="C243" s="3">
         <v>0.12</v>
       </c>
-      <c r="D243" s="64" t="s">
+      <c r="D243" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E243" s="65" t="s">
+      <c r="E243" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F243" s="64" t="s">
+      <c r="F243" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12332,9 +12360,9 @@
       <c r="C244" s="3">
         <v>0.12</v>
       </c>
-      <c r="D244" s="64"/>
-      <c r="E244" s="66"/>
-      <c r="F244" s="64"/>
+      <c r="D244" s="66"/>
+      <c r="E244" s="65"/>
+      <c r="F244" s="66"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" s="8" t="s">
@@ -12424,13 +12452,13 @@
       <c r="C254" s="3">
         <v>0.12</v>
       </c>
-      <c r="D254" s="64" t="s">
+      <c r="D254" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E254" s="65" t="s">
+      <c r="E254" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F254" s="64" t="s">
+      <c r="F254" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12442,9 +12470,9 @@
       <c r="C255" s="3">
         <v>0.12</v>
       </c>
-      <c r="D255" s="64"/>
-      <c r="E255" s="66"/>
-      <c r="F255" s="64"/>
+      <c r="D255" s="66"/>
+      <c r="E255" s="65"/>
+      <c r="F255" s="66"/>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256" s="8" t="s">
@@ -12487,49 +12515,21 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="E151:E152"/>
-    <mergeCell ref="F151:F152"/>
-    <mergeCell ref="D185:D186"/>
-    <mergeCell ref="E185:E186"/>
-    <mergeCell ref="F185:F186"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="D173:D174"/>
-    <mergeCell ref="E173:E174"/>
-    <mergeCell ref="F173:F174"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="D254:D255"/>
+    <mergeCell ref="E254:E255"/>
+    <mergeCell ref="F254:F255"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="E232:E233"/>
+    <mergeCell ref="F232:F233"/>
+    <mergeCell ref="D243:D244"/>
+    <mergeCell ref="E243:E244"/>
+    <mergeCell ref="F243:F244"/>
+    <mergeCell ref="D210:D211"/>
+    <mergeCell ref="E210:E211"/>
+    <mergeCell ref="F210:F211"/>
+    <mergeCell ref="D221:D222"/>
+    <mergeCell ref="E221:E222"/>
+    <mergeCell ref="F221:F222"/>
     <mergeCell ref="D197:D198"/>
     <mergeCell ref="E197:E198"/>
     <mergeCell ref="F197:F198"/>
@@ -12546,21 +12546,49 @@
     <mergeCell ref="E140:E141"/>
     <mergeCell ref="F140:F141"/>
     <mergeCell ref="D151:D152"/>
-    <mergeCell ref="D210:D211"/>
-    <mergeCell ref="E210:E211"/>
-    <mergeCell ref="F210:F211"/>
-    <mergeCell ref="D221:D222"/>
-    <mergeCell ref="E221:E222"/>
-    <mergeCell ref="F221:F222"/>
-    <mergeCell ref="D254:D255"/>
-    <mergeCell ref="E254:E255"/>
-    <mergeCell ref="F254:F255"/>
-    <mergeCell ref="D232:D233"/>
-    <mergeCell ref="E232:E233"/>
-    <mergeCell ref="F232:F233"/>
-    <mergeCell ref="D243:D244"/>
-    <mergeCell ref="E243:E244"/>
-    <mergeCell ref="F243:F244"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="E151:E152"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="D185:D186"/>
+    <mergeCell ref="E185:E186"/>
+    <mergeCell ref="F185:F186"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="D173:D174"/>
+    <mergeCell ref="E173:E174"/>
+    <mergeCell ref="F173:F174"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12689,13 +12717,13 @@
       <c r="C5" s="3">
         <v>0.12</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="1"/>
@@ -12705,13 +12733,13 @@
       <c r="K5" s="3">
         <v>0.12</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="65" t="s">
+      <c r="M5" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="64" t="s">
+      <c r="N5" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12723,9 +12751,9 @@
       <c r="C6" s="3">
         <v>0.12</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="64"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="66"/>
       <c r="I6" s="1"/>
       <c r="J6" s="28" t="s">
         <v>10</v>
@@ -12733,9 +12761,9 @@
       <c r="K6" s="3">
         <v>0.12</v>
       </c>
-      <c r="L6" s="64"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="64"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="66"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -12895,13 +12923,13 @@
       <c r="C16" s="3">
         <v>0.12</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I16" s="1"/>
@@ -12911,13 +12939,13 @@
       <c r="K16" s="3">
         <v>0.12</v>
       </c>
-      <c r="L16" s="64" t="s">
+      <c r="L16" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="65" t="s">
+      <c r="M16" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="64" t="s">
+      <c r="N16" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -12929,9 +12957,9 @@
       <c r="C17" s="3">
         <v>0.12</v>
       </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="64"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="66"/>
       <c r="I17" s="1"/>
       <c r="J17" s="28" t="s">
         <v>10</v>
@@ -12939,9 +12967,9 @@
       <c r="K17" s="3">
         <v>0.12</v>
       </c>
-      <c r="L17" s="64"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="64"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="65"/>
+      <c r="N17" s="66"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
@@ -13101,13 +13129,13 @@
       <c r="C27" s="3">
         <v>0.12</v>
       </c>
-      <c r="D27" s="64" t="s">
+      <c r="D27" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="65" t="s">
+      <c r="E27" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="64" t="s">
+      <c r="F27" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I27" s="1"/>
@@ -13117,13 +13145,13 @@
       <c r="K27" s="3">
         <v>0.12</v>
       </c>
-      <c r="L27" s="64" t="s">
+      <c r="L27" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M27" s="65" t="s">
+      <c r="M27" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N27" s="64" t="s">
+      <c r="N27" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13135,9 +13163,9 @@
       <c r="C28" s="3">
         <v>0.12</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="64"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
       <c r="I28" s="1"/>
       <c r="J28" s="28" t="s">
         <v>10</v>
@@ -13145,9 +13173,9 @@
       <c r="K28" s="3">
         <v>0.12</v>
       </c>
-      <c r="L28" s="64"/>
-      <c r="M28" s="66"/>
-      <c r="N28" s="64"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="66"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
@@ -13307,13 +13335,13 @@
       <c r="C38" s="3">
         <v>0.12</v>
       </c>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="65" t="s">
+      <c r="E38" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="64" t="s">
+      <c r="F38" s="66" t="s">
         <v>31</v>
       </c>
       <c r="I38" s="1"/>
@@ -13323,13 +13351,13 @@
       <c r="K38" s="3">
         <v>0.12</v>
       </c>
-      <c r="L38" s="64" t="s">
+      <c r="L38" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="M38" s="65" t="s">
+      <c r="M38" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="N38" s="64" t="s">
+      <c r="N38" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13341,9 +13369,9 @@
       <c r="C39" s="3">
         <v>0.12</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="64"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="66"/>
       <c r="I39" s="1"/>
       <c r="J39" s="28" t="s">
         <v>10</v>
@@ -13351,9 +13379,9 @@
       <c r="K39" s="3">
         <v>0.12</v>
       </c>
-      <c r="L39" s="64"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="64"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="65"/>
+      <c r="N39" s="66"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
@@ -13489,13 +13517,13 @@
       <c r="C50" s="3">
         <v>0.12</v>
       </c>
-      <c r="D50" s="64" t="s">
+      <c r="D50" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="65" t="s">
+      <c r="E50" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="64" t="s">
+      <c r="F50" s="66" t="s">
         <v>31</v>
       </c>
       <c r="G50" s="39"/>
@@ -13511,9 +13539,9 @@
       <c r="C51" s="3">
         <v>0.12</v>
       </c>
-      <c r="D51" s="64"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="64"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="66"/>
       <c r="G51" s="39"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -13614,13 +13642,13 @@
       <c r="C61" s="3">
         <v>0.12</v>
       </c>
-      <c r="D61" s="64" t="s">
+      <c r="D61" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="E61" s="65" t="s">
+      <c r="E61" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="64" t="s">
+      <c r="F61" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -13632,9 +13660,9 @@
       <c r="C62" s="3">
         <v>0.12</v>
       </c>
-      <c r="D62" s="64"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="64"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="66"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
@@ -13679,6 +13707,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="N27:N28"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="E50:E51"/>
     <mergeCell ref="F50:F51"/>
@@ -13695,22 +13739,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13720,8 +13748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15186,10 +15214,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15216,11 +15244,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
       <c r="D1" s="1" t="s">
         <v>141</v>
       </c>
@@ -15230,22 +15258,22 @@
       <c r="G1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="74"/>
-      <c r="K1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="76"/>
       <c r="L1" s="1" t="s">
         <v>141</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
       <c r="U1" s="1" t="s">
         <v>141</v>
       </c>
@@ -15365,13 +15393,13 @@
       <c r="C4" s="70">
         <v>11.41</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="66">
         <v>747</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="64">
         <v>37753</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="66" t="s">
         <v>31</v>
       </c>
       <c r="G4" t="s">
@@ -15385,13 +15413,13 @@
         <f>(M4/M2)*100</f>
         <v>11.833364075365353</v>
       </c>
-      <c r="L4" s="64">
+      <c r="L4" s="66">
         <v>747</v>
       </c>
-      <c r="M4" s="65">
+      <c r="M4" s="64">
         <v>39134</v>
       </c>
-      <c r="N4" s="64" t="s">
+      <c r="N4" s="66" t="s">
         <v>31</v>
       </c>
       <c r="R4" s="8" t="s">
@@ -15402,13 +15430,13 @@
         <f>(V4/V2)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U4" s="64">
+      <c r="U4" s="66">
         <v>747</v>
       </c>
-      <c r="V4" s="65">
+      <c r="V4" s="64">
         <v>49060</v>
       </c>
-      <c r="W4" s="64" t="s">
+      <c r="W4" s="66" t="s">
         <v>31</v>
       </c>
       <c r="X4" t="s">
@@ -15423,9 +15451,9 @@
         <v>108</v>
       </c>
       <c r="C5" s="71"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="64"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="66"/>
       <c r="G5" t="s">
         <v>155</v>
       </c>
@@ -15436,9 +15464,9 @@
         <v>108</v>
       </c>
       <c r="K5" s="71"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="64"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="66"/>
       <c r="R5" s="13" t="s">
         <v>12</v>
       </c>
@@ -15446,9 +15474,9 @@
         <v>108</v>
       </c>
       <c r="T5" s="71"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="64"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="66"/>
       <c r="X5" t="s">
         <v>155</v>
       </c>
@@ -15693,13 +15721,13 @@
       <c r="C15" s="28">
         <v>11.41</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="66">
         <v>747</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="64">
         <v>37753</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="72" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="54" t="s">
@@ -15713,13 +15741,13 @@
         <f>(V15/V13)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U15" s="64">
+      <c r="U15" s="66">
         <v>747</v>
       </c>
-      <c r="V15" s="65">
+      <c r="V15" s="64">
         <v>49060</v>
       </c>
-      <c r="W15" s="64" t="s">
+      <c r="W15" s="66" t="s">
         <v>31</v>
       </c>
       <c r="X15" t="s">
@@ -15736,9 +15764,9 @@
       <c r="C16" s="28">
         <v>11.41</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="76"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="72"/>
       <c r="G16" s="54" t="s">
         <v>156</v>
       </c>
@@ -15749,9 +15777,9 @@
         <v>108</v>
       </c>
       <c r="T16" s="71"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="66"/>
-      <c r="W16" s="64"/>
+      <c r="U16" s="66"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="66"/>
       <c r="X16" t="s">
         <v>155</v>
       </c>
@@ -16006,10 +16034,10 @@
         <f>(V27/V25)*100</f>
         <v>11.829040704823722</v>
       </c>
-      <c r="U27" s="64">
+      <c r="U27" s="66">
         <v>747</v>
       </c>
-      <c r="V27" s="65">
+      <c r="V27" s="64">
         <v>49060</v>
       </c>
       <c r="X27" t="s">
@@ -16026,13 +16054,13 @@
       <c r="C28" s="28">
         <v>11.41</v>
       </c>
-      <c r="D28" s="64">
+      <c r="D28" s="66">
         <v>747</v>
       </c>
-      <c r="E28" s="65">
+      <c r="E28" s="64">
         <v>37753</v>
       </c>
-      <c r="F28" s="76" t="s">
+      <c r="F28" s="72" t="s">
         <v>31</v>
       </c>
       <c r="G28" s="58"/>
@@ -16043,8 +16071,8 @@
         <v>108</v>
       </c>
       <c r="T28" s="71"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="66"/>
+      <c r="U28" s="66"/>
+      <c r="V28" s="65"/>
       <c r="X28" t="s">
         <v>155</v>
       </c>
@@ -16059,9 +16087,9 @@
       <c r="C29" s="28">
         <v>11.41</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="76"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="72"/>
       <c r="G29" s="58"/>
       <c r="R29" s="13" t="s">
         <v>22</v>
@@ -16262,10 +16290,10 @@
         <f>(V37/V35)*100</f>
         <v>11.415776407657487</v>
       </c>
-      <c r="U37" s="64">
+      <c r="U37" s="66">
         <v>747</v>
       </c>
-      <c r="V37" s="65">
+      <c r="V37" s="64">
         <v>37753</v>
       </c>
       <c r="X37" t="s">
@@ -16279,8 +16307,8 @@
       </c>
       <c r="S38" s="30"/>
       <c r="T38" s="71"/>
-      <c r="U38" s="64"/>
-      <c r="V38" s="66"/>
+      <c r="U38" s="66"/>
+      <c r="V38" s="65"/>
       <c r="X38" t="s">
         <v>155</v>
       </c>
@@ -16349,13 +16377,13 @@
       <c r="C41" s="28">
         <v>11.41</v>
       </c>
-      <c r="D41" s="64">
+      <c r="D41" s="66">
         <v>747</v>
       </c>
-      <c r="E41" s="65">
+      <c r="E41" s="64">
         <v>37753</v>
       </c>
-      <c r="F41" s="76" t="s">
+      <c r="F41" s="72" t="s">
         <v>31</v>
       </c>
       <c r="G41" s="58"/>
@@ -16377,9 +16405,9 @@
       <c r="C42" s="28">
         <v>11.41</v>
       </c>
-      <c r="D42" s="64"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="76"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="72"/>
       <c r="G42" s="58"/>
       <c r="R42" s="13" t="s">
         <v>132</v>
@@ -16520,10 +16548,10 @@
         <f>(V48/V46)*100</f>
         <v>11.415776407657487</v>
       </c>
-      <c r="U48" s="64">
+      <c r="U48" s="66">
         <v>747</v>
       </c>
-      <c r="V48" s="65">
+      <c r="V48" s="64">
         <v>37753</v>
       </c>
     </row>
@@ -16548,8 +16576,8 @@
       </c>
       <c r="S49" s="30"/>
       <c r="T49" s="71"/>
-      <c r="U49" s="64"/>
-      <c r="V49" s="66"/>
+      <c r="U49" s="66"/>
+      <c r="V49" s="65"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C50" s="58"/>
@@ -16564,10 +16592,18 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
+      <c r="A51" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="26">
+        <v>41</v>
+      </c>
+      <c r="D51" s="1">
+        <v>6236</v>
+      </c>
+      <c r="E51" s="1">
+        <v>330709</v>
+      </c>
       <c r="R51" s="13" t="s">
         <v>24</v>
       </c>
@@ -16576,6 +16612,21 @@
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="28">
+        <v>88.5</v>
+      </c>
+      <c r="D52" s="2">
+        <v>5489</v>
+      </c>
+      <c r="E52" s="2">
+        <v>292956</v>
+      </c>
       <c r="R52" s="13" t="s">
         <v>42</v>
       </c>
@@ -16584,6 +16635,24 @@
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="77">
+        <v>4</v>
+      </c>
+      <c r="C53" s="28">
+        <v>11.41</v>
+      </c>
+      <c r="D53" s="66">
+        <v>747</v>
+      </c>
+      <c r="E53" s="64">
+        <v>37753</v>
+      </c>
+      <c r="F53" s="72" t="s">
+        <v>31</v>
+      </c>
       <c r="R53" s="13" t="s">
         <v>132</v>
       </c>
@@ -16593,6 +16662,16 @@
       <c r="T53" s="22"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="30"/>
+      <c r="C54" s="28">
+        <v>11.41</v>
+      </c>
+      <c r="D54" s="66"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="72"/>
       <c r="R54" s="48" t="s">
         <v>142</v>
       </c>
@@ -16601,7 +16680,27 @@
       </c>
       <c r="T54" s="22"/>
     </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" t="s">
+        <v>136</v>
+      </c>
+    </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>162</v>
+      </c>
       <c r="R56" s="21" t="s">
         <v>11</v>
       </c>
@@ -16619,6 +16718,12 @@
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A57" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="R57" s="6" t="s">
         <v>0</v>
       </c>
@@ -16637,6 +16742,16 @@
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="C58" s="62"/>
+      <c r="D58" s="58"/>
+      <c r="E58" s="58"/>
+      <c r="F58" s="58"/>
       <c r="R58" s="8" t="s">
         <v>4</v>
       </c>
@@ -16645,23 +16760,49 @@
         <f>(V58/V56)*100</f>
         <v>11.415776407657487</v>
       </c>
-      <c r="U58" s="64">
+      <c r="U58" s="66">
         <v>747</v>
       </c>
-      <c r="V58" s="65">
+      <c r="V58" s="64">
         <v>37753</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A59" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="58"/>
+      <c r="D59" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="E59" s="46"/>
+      <c r="F59" s="58"/>
       <c r="R59" s="13" t="s">
         <v>12</v>
       </c>
       <c r="S59" s="30"/>
       <c r="T59" s="71"/>
-      <c r="U59" s="64"/>
-      <c r="V59" s="66"/>
+      <c r="U59" s="66"/>
+      <c r="V59" s="65"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B60" s="61">
+        <v>1528</v>
+      </c>
+      <c r="C60" s="62"/>
+      <c r="D60" s="46">
+        <v>1733</v>
+      </c>
+      <c r="E60" s="57">
+        <v>4.5900000000000003E-2</v>
+      </c>
+      <c r="F60" s="58"/>
       <c r="R60" s="13" t="s">
         <v>22</v>
       </c>
@@ -16670,6 +16811,20 @@
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A61" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" s="61">
+        <v>964</v>
+      </c>
+      <c r="C61" s="62"/>
+      <c r="D61" s="46">
+        <v>1169</v>
+      </c>
+      <c r="E61" s="57">
+        <v>3.09E-2</v>
+      </c>
+      <c r="F61" s="58"/>
       <c r="R61" s="13" t="s">
         <v>24</v>
       </c>
@@ -16704,16 +16859,26 @@
       <c r="T64" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="V48:V49"/>
-    <mergeCell ref="T58:T59"/>
-    <mergeCell ref="U58:U59"/>
-    <mergeCell ref="V58:V59"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="T48:T49"/>
-    <mergeCell ref="U48:U49"/>
+  <mergeCells count="43">
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="T27:T28"/>
+    <mergeCell ref="U27:U28"/>
+    <mergeCell ref="V27:V28"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="V37:V38"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="E15:E16"/>
@@ -16726,25 +16891,18 @@
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="T27:T28"/>
-    <mergeCell ref="U27:U28"/>
-    <mergeCell ref="V27:V28"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="V48:V49"/>
+    <mergeCell ref="T58:T59"/>
+    <mergeCell ref="U58:U59"/>
+    <mergeCell ref="V58:V59"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="T48:T49"/>
+    <mergeCell ref="U48:U49"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>